<commit_message>
Update SEO analysis document
</commit_message>
<xml_diff>
--- a/Modele-audit-SEO.xlsx
+++ b/Modele-audit-SEO.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
   <si>
     <t>Catégorie</t>
   </si>
@@ -97,6 +97,69 @@
     <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055236-parametrez-le-cache-navigateur</t>
   </si>
   <si>
+    <t>Présence de "keywords spammy"</t>
+  </si>
+  <si>
+    <t>Des mots clés sont cachés sur la page et doivent être enlevés car cela constitue une technique pénalisé par les moteur de recherche</t>
+  </si>
+  <si>
+    <t>Ne pas utiliser de technique black hat sur les pages et donc éviter de répéter un mot clé abusivement et de cacher du texte sur la page. Le contenu doit primé sur le reste</t>
+  </si>
+  <si>
+    <t>Supprimer le contenu succeptible d'être considéré comme une tricherie par les moteurs de recherche</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/search/docs/advanced/guidelines/irrelevant-keywords?hl=fr</t>
+  </si>
+  <si>
+    <t>Image contenant juste un texte</t>
+  </si>
+  <si>
+    <t>Ces images ont 2 inconvénients, elles prennent plus de temps à charger que le texte et ne permettent pas aux moteurs de recherche d'analyser le contenu du texte. Ceci nuit donc aux performances et au contenu de la page</t>
+  </si>
+  <si>
+    <t>Ne pas utiliser d'image pourafficher un simple texte sur les pages</t>
+  </si>
+  <si>
+    <t>Ajouter et mettre en forme le texte contenu dans les image pour les remplacer</t>
+  </si>
+  <si>
+    <t>https://www.dummies.com/web-design-development/search-engine-optimization/avoid-embedded-text-in-images-for-seo/</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>Le texte alternatif à certaines images est manquant ou inadéquat</t>
+  </si>
+  <si>
+    <t>L'absence de texte alternatif prive les utilisateur non voyants d'information véhiculées par l'image</t>
+  </si>
+  <si>
+    <t>Toujours fournir un texte alternatif descriptif pour les images</t>
+  </si>
+  <si>
+    <t>Ajouter un texte alternatif aux images</t>
+  </si>
+  <si>
+    <t>https://www.alsacreations.com/astuce/lire/1166-alt-title-images-liens.html</t>
+  </si>
+  <si>
+    <t>aria-label manquant sur les liens sans texte</t>
+  </si>
+  <si>
+    <t>Un lien sans texte ne fourni pas d'information sur ce sur quoi il pointe pour aux visiteur ne pouvant pas voir les images</t>
+  </si>
+  <si>
+    <t>Lorsque qu'un lien est composé uniquement d'une image, il est impératif de lui fournir un label afin que les robots et les lecteurs d'écran savent vers où il pointe</t>
+  </si>
+  <si>
+    <t>Ajouter un label aux liens ne comportant qu'une image</t>
+  </si>
+  <si>
+    <t>https://www.aditus.io/aria/aria-label/</t>
+  </si>
+  <si>
     <t>Outils de mesure non installés</t>
   </si>
   <si>
@@ -112,16 +175,16 @@
     <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5604431-installez-les-bons-outils</t>
   </si>
   <si>
-    <t>Balise meta robots manquante</t>
-  </si>
-  <si>
-    <t>En l'absense de balise meta robots on ne peut paramétrer le comportement du robot face à no pages</t>
-  </si>
-  <si>
-    <t>Demander au robots d'indexer et de crawler dean les pages ou c'est prévu</t>
-  </si>
-  <si>
-    <t>Ajouter les balises meta robots</t>
+    <t>robots.txt et sitemap.txt manquants</t>
+  </si>
+  <si>
+    <t>En l'absense de ces fichiers on ne peut paramétrer le comportement du robot face à nos pages</t>
+  </si>
+  <si>
+    <t>Demander au robots d'indexer et de crawler dans les pages ou c'est prévu via ces fichiers</t>
+  </si>
+  <si>
+    <t>Ajouter le robots.txt et le sitemap.txt</t>
   </si>
   <si>
     <t>https://www.webrankinfo.com/dossiers/conseils/balise-meta-robots#:~:text=Meta%20robots%20%3A%20d%C3%A9finition%20et%20code%20HTML&amp;text=La%20meta%20meta%20robots%20est,la%20page%20(robots%20noindex).</t>
@@ -133,7 +196,7 @@
     <t>Certains des liens sur la page sont mort ou pointe vers des sites non pertinents</t>
   </si>
   <si>
-    <t>Purgr les liens sur la page</t>
+    <t>Purger les liens sur la page</t>
   </si>
   <si>
     <t>Enlever les liens morts ainsi que les liens vers des sites sans rapport avec notre activité</t>
@@ -155,10 +218,10 @@
     <t>Absence de données structurées</t>
   </si>
   <si>
-    <t>Le site ne fournit pas de données structurées</t>
-  </si>
-  <si>
-    <t>Autant que possible utiliser les donénes structurées</t>
+    <t>Le site ne fournit pas de données structurées ce qui ne prive les outils d'analyse (notamment des réseaux sociaux) d'obtenir des meta informations pertinentes sur le contenu</t>
+  </si>
+  <si>
+    <t>Autant que possible utiliser les données structurées afin d'améliorer la prise en charge par les systèmes d'analyses</t>
   </si>
   <si>
     <t>Ajouter des données structurées pour décrire le contenu</t>
@@ -167,10 +230,10 @@
     <t>https://developers.google.com/search/docs/guides/intro-structured-data?hl=fr</t>
   </si>
   <si>
-    <t>Ajouter no follow sur les liens du footer</t>
-  </si>
-  <si>
-    <t>Trop de lien no tagué no follow et donne une image peu qualitative à la page</t>
+    <t>Liens dupliqués</t>
+  </si>
+  <si>
+    <t>Trop de liens dupliqués non tagués no follow et donne une image peu qualitative à la page</t>
   </si>
   <si>
     <t>penser à réduire le nombre de lien et les taguer en nofollow s'ils ne sont pas en lien avec le contenu</t>
@@ -206,47 +269,20 @@
     <t>Déterminer le type de contenu qui améliorerait la cohérence du site et sa visibilité et mettre en place les outils et le processus de création de ce contenus</t>
   </si>
   <si>
-    <t>ajouter des pages pour décrire les porojets menés à bien</t>
+    <t>ajouter des pages pour décrire les projets menés à bien et mettre en place un système pour faciliter la génération du contenu</t>
   </si>
   <si>
     <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578344-creez-votre-machine-a-contenu</t>
   </si>
   <si>
-    <t>Présence de "keywords spammy"</t>
-  </si>
-  <si>
-    <t>Des mots clés sont cachés sur la page et doivent être enlevés car cela constitue une technique pénalisé par les moteur de recherche</t>
-  </si>
-  <si>
-    <t>Ne pas utiliser de technique black hat sur les pages et donc éviter de répéter un mot clé abusivement et de cacher du texte sur la page. Le contenu doit primé sur le reste</t>
-  </si>
-  <si>
-    <t>Supprimer le contenu succeptible d'être considéré comme une tricherie par les moteurs de recherche</t>
-  </si>
-  <si>
-    <t>https://developers.google.com/search/docs/advanced/guidelines/irrelevant-keywords?hl=fr</t>
-  </si>
-  <si>
-    <t>Image contenant juste un texte</t>
-  </si>
-  <si>
-    <t>Ces images ont 2 inconvénients, elles prennent plus de temps à charger que le texte et ne permettent pas aux moteurs de recherche d'analyser le contenu du texte. Ceci nuit donc aux performances et au contenu de la page</t>
-  </si>
-  <si>
-    <t>Ne pas utiliser d'image pourafficher un simple texte sur les pages</t>
-  </si>
-  <si>
-    <t>Ajouter et mettre en forme le texte contenu dans les image pour les remplacer</t>
-  </si>
-  <si>
-    <t>https://www.dummies.com/web-design-development/search-engine-optimization/avoid-embedded-text-in-images-for-seo/</t>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -268,6 +304,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -290,6 +327,14 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -306,8 +351,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFB4A7D6"/>
+        <bgColor rgb="FFB4A7D6"/>
       </patternFill>
     </fill>
   </fills>
@@ -328,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -339,6 +384,24 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -348,17 +411,16 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -582,7 +644,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="13.33"/>
     <col customWidth="1" min="2" max="2" width="39.0"/>
-    <col customWidth="1" min="3" max="3" width="43.11"/>
+    <col customWidth="1" min="3" max="3" width="34.22"/>
     <col customWidth="1" min="4" max="4" width="36.78"/>
     <col customWidth="1" min="5" max="5" width="41.0"/>
     <col customWidth="1" min="6" max="6" width="86.33"/>
@@ -635,22 +697,22 @@
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -658,22 +720,22 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -681,22 +743,22 @@
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -704,22 +766,22 @@
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -727,3167 +789,3209 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="4">
-        <v>1.0</v>
+      <c r="G6" s="5">
+        <v>0.0</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="4">
-        <v>1.0</v>
+      <c r="G7" s="5">
+        <v>0.0</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="4">
-        <v>1.0</v>
+      <c r="F8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.0</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="E9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="4">
-        <v>1.0</v>
+      <c r="F9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="4">
+      <c r="F10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="4">
+      <c r="F11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="10">
         <v>2.0</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="4" t="s">
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="4">
+      <c r="B16" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="10">
         <v>2.0</v>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="E15" s="11"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="10"/>
-    </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="10"/>
+      <c r="A17" s="16"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="10"/>
+      <c r="A18" s="16"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="10"/>
+      <c r="A19" s="16"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="10"/>
+      <c r="A20" s="16"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="10"/>
+      <c r="A21" s="16"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="10"/>
+      <c r="A22" s="16"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="10"/>
+      <c r="A23" s="16"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="10"/>
+      <c r="A24" s="16"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="10"/>
+      <c r="A25" s="16"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="10"/>
+      <c r="A26" s="16"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="10"/>
+      <c r="A27" s="16"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="10"/>
+      <c r="A28" s="16"/>
+      <c r="C28" s="10" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="10"/>
+      <c r="A29" s="16"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="10"/>
+      <c r="A30" s="16"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="10"/>
+      <c r="A31" s="16"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="10"/>
+      <c r="A32" s="16"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="10"/>
+      <c r="A33" s="16"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="10"/>
+      <c r="A34" s="16"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="10"/>
+      <c r="A35" s="16"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="10"/>
+      <c r="A36" s="16"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="10"/>
+      <c r="A37" s="16"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="10"/>
+      <c r="A38" s="16"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="10"/>
+      <c r="A39" s="16"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="10"/>
+      <c r="A40" s="16"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="10"/>
+      <c r="A41" s="16"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="10"/>
+      <c r="A42" s="16"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="10"/>
+      <c r="A43" s="16"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="10"/>
+      <c r="A44" s="16"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="10"/>
+      <c r="A45" s="16"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="10"/>
+      <c r="A46" s="16"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="10"/>
+      <c r="A47" s="16"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="10"/>
+      <c r="A48" s="16"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="10"/>
+      <c r="A49" s="16"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="10"/>
+      <c r="A50" s="16"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="10"/>
+      <c r="A51" s="16"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="10"/>
+      <c r="A52" s="16"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="10"/>
+      <c r="A53" s="16"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="10"/>
+      <c r="A54" s="16"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="10"/>
+      <c r="A55" s="16"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="10"/>
+      <c r="A56" s="16"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="10"/>
+      <c r="A57" s="16"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="10"/>
+      <c r="A58" s="16"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="10"/>
+      <c r="A59" s="16"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="10"/>
+      <c r="A60" s="16"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="10"/>
+      <c r="A61" s="16"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="10"/>
+      <c r="A62" s="16"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="10"/>
+      <c r="A63" s="16"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="10"/>
+      <c r="A64" s="16"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="10"/>
+      <c r="A65" s="16"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="10"/>
+      <c r="A66" s="16"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="10"/>
+      <c r="A67" s="16"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="10"/>
+      <c r="A68" s="16"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="10"/>
+      <c r="A69" s="16"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="10"/>
+      <c r="A70" s="16"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="10"/>
+      <c r="A71" s="16"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="10"/>
+      <c r="A72" s="16"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="10"/>
+      <c r="A73" s="16"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="10"/>
+      <c r="A74" s="16"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="10"/>
+      <c r="A75" s="16"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="10"/>
+      <c r="A76" s="16"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="10"/>
+      <c r="A77" s="16"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="10"/>
+      <c r="A78" s="16"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="10"/>
+      <c r="A79" s="16"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="10"/>
+      <c r="A80" s="16"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="10"/>
+      <c r="A81" s="16"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="10"/>
+      <c r="A82" s="16"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="10"/>
+      <c r="A83" s="16"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="10"/>
+      <c r="A84" s="16"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="10"/>
+      <c r="A85" s="16"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="10"/>
+      <c r="A86" s="16"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="10"/>
+      <c r="A87" s="16"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="10"/>
+      <c r="A88" s="16"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="10"/>
+      <c r="A89" s="16"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="10"/>
+      <c r="A90" s="16"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="10"/>
+      <c r="A91" s="16"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="10"/>
+      <c r="A92" s="16"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="10"/>
+      <c r="A93" s="16"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="10"/>
+      <c r="A94" s="16"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="10"/>
+      <c r="A95" s="16"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="10"/>
+      <c r="A96" s="16"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="10"/>
+      <c r="A97" s="16"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="10"/>
+      <c r="A98" s="16"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="10"/>
+      <c r="A99" s="16"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="10"/>
+      <c r="A100" s="16"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="10"/>
+      <c r="A101" s="16"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="10"/>
+      <c r="A102" s="16"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="10"/>
+      <c r="A103" s="16"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="10"/>
+      <c r="A104" s="16"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="10"/>
+      <c r="A105" s="16"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="10"/>
+      <c r="A106" s="16"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="10"/>
+      <c r="A107" s="16"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="10"/>
+      <c r="A108" s="16"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="10"/>
+      <c r="A109" s="16"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="10"/>
+      <c r="A110" s="16"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="10"/>
+      <c r="A111" s="16"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="10"/>
+      <c r="A112" s="16"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="10"/>
+      <c r="A113" s="16"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="10"/>
+      <c r="A114" s="16"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="10"/>
+      <c r="A115" s="16"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="10"/>
+      <c r="A116" s="16"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="10"/>
+      <c r="A117" s="16"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="10"/>
+      <c r="A118" s="16"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="10"/>
+      <c r="A119" s="16"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="10"/>
+      <c r="A120" s="16"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="10"/>
+      <c r="A121" s="16"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="10"/>
+      <c r="A122" s="16"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="10"/>
+      <c r="A123" s="16"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="10"/>
+      <c r="A124" s="16"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="10"/>
+      <c r="A125" s="16"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="10"/>
+      <c r="A126" s="16"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="10"/>
+      <c r="A127" s="16"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="10"/>
+      <c r="A128" s="16"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="10"/>
+      <c r="A129" s="16"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="10"/>
+      <c r="A130" s="16"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="10"/>
+      <c r="A131" s="16"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="10"/>
+      <c r="A132" s="16"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="10"/>
+      <c r="A133" s="16"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="10"/>
+      <c r="A134" s="16"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="10"/>
+      <c r="A135" s="16"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="10"/>
+      <c r="A136" s="16"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="10"/>
+      <c r="A137" s="16"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="10"/>
+      <c r="A138" s="16"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="10"/>
+      <c r="A139" s="16"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="10"/>
+      <c r="A140" s="16"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="10"/>
+      <c r="A141" s="16"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="10"/>
+      <c r="A142" s="16"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="10"/>
+      <c r="A143" s="16"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="10"/>
+      <c r="A144" s="16"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="10"/>
+      <c r="A145" s="16"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="10"/>
+      <c r="A146" s="16"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="10"/>
+      <c r="A147" s="16"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="10"/>
+      <c r="A148" s="16"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="10"/>
+      <c r="A149" s="16"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="10"/>
+      <c r="A150" s="16"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="10"/>
+      <c r="A151" s="16"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="10"/>
+      <c r="A152" s="16"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="10"/>
+      <c r="A153" s="16"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="10"/>
+      <c r="A154" s="16"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="10"/>
+      <c r="A155" s="16"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="10"/>
+      <c r="A156" s="16"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="10"/>
+      <c r="A157" s="16"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="10"/>
+      <c r="A158" s="16"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="10"/>
+      <c r="A159" s="16"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="10"/>
+      <c r="A160" s="16"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="10"/>
+      <c r="A161" s="16"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="10"/>
+      <c r="A162" s="16"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="10"/>
+      <c r="A163" s="16"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="10"/>
+      <c r="A164" s="16"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="10"/>
+      <c r="A165" s="16"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="10"/>
+      <c r="A166" s="16"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="10"/>
+      <c r="A167" s="16"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="10"/>
+      <c r="A168" s="16"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="10"/>
+      <c r="A169" s="16"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="10"/>
+      <c r="A170" s="16"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="10"/>
+      <c r="A171" s="16"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="10"/>
+      <c r="A172" s="16"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="10"/>
+      <c r="A173" s="16"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="10"/>
+      <c r="A174" s="16"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="10"/>
+      <c r="A175" s="16"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="10"/>
+      <c r="A176" s="16"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="10"/>
+      <c r="A177" s="16"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="10"/>
+      <c r="A178" s="16"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="10"/>
+      <c r="A179" s="16"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="10"/>
+      <c r="A180" s="16"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="10"/>
+      <c r="A181" s="16"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="10"/>
+      <c r="A182" s="16"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="10"/>
+      <c r="A183" s="16"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="10"/>
+      <c r="A184" s="16"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="10"/>
+      <c r="A185" s="16"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="10"/>
+      <c r="A186" s="16"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="10"/>
+      <c r="A187" s="16"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="10"/>
+      <c r="A188" s="16"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="10"/>
+      <c r="A189" s="16"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="10"/>
+      <c r="A190" s="16"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="10"/>
+      <c r="A191" s="16"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="10"/>
+      <c r="A192" s="16"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="10"/>
+      <c r="A193" s="16"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="10"/>
+      <c r="A194" s="16"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="10"/>
+      <c r="A195" s="16"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="10"/>
+      <c r="A196" s="16"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="10"/>
+      <c r="A197" s="16"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="10"/>
+      <c r="A198" s="16"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="10"/>
+      <c r="A199" s="16"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="10"/>
+      <c r="A200" s="16"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="10"/>
+      <c r="A201" s="16"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="10"/>
+      <c r="A202" s="16"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="10"/>
+      <c r="A203" s="16"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="10"/>
+      <c r="A204" s="16"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="10"/>
+      <c r="A205" s="16"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="10"/>
+      <c r="A206" s="16"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="10"/>
+      <c r="A207" s="16"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="10"/>
+      <c r="A208" s="16"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="10"/>
+      <c r="A209" s="16"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="10"/>
+      <c r="A210" s="16"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="10"/>
+      <c r="A211" s="16"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="10"/>
+      <c r="A212" s="16"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="10"/>
+      <c r="A213" s="16"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="10"/>
+      <c r="A214" s="16"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="10"/>
+      <c r="A215" s="16"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="10"/>
+      <c r="A216" s="16"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="10"/>
+      <c r="A217" s="16"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="10"/>
+      <c r="A218" s="16"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="10"/>
+      <c r="A219" s="16"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="10"/>
+      <c r="A220" s="16"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="10"/>
+      <c r="A221" s="16"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="10"/>
+      <c r="A222" s="16"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="10"/>
+      <c r="A223" s="16"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="10"/>
+      <c r="A224" s="16"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="10"/>
+      <c r="A225" s="16"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="10"/>
+      <c r="A226" s="16"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="10"/>
+      <c r="A227" s="16"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="10"/>
+      <c r="A228" s="16"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="10"/>
+      <c r="A229" s="16"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="A230" s="10"/>
+      <c r="A230" s="16"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="A231" s="10"/>
+      <c r="A231" s="16"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="10"/>
+      <c r="A232" s="16"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="A233" s="10"/>
+      <c r="A233" s="16"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="A234" s="10"/>
+      <c r="A234" s="16"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="A235" s="10"/>
+      <c r="A235" s="16"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="10"/>
+      <c r="A236" s="16"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="10"/>
+      <c r="A237" s="16"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="10"/>
+      <c r="A238" s="16"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="A239" s="10"/>
+      <c r="A239" s="16"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="A240" s="10"/>
+      <c r="A240" s="16"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="A241" s="10"/>
+      <c r="A241" s="16"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="A242" s="10"/>
+      <c r="A242" s="16"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="A243" s="10"/>
+      <c r="A243" s="16"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="A244" s="10"/>
+      <c r="A244" s="16"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="A245" s="10"/>
+      <c r="A245" s="16"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="A246" s="10"/>
+      <c r="A246" s="16"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="A247" s="10"/>
+      <c r="A247" s="16"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="A248" s="10"/>
+      <c r="A248" s="16"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="A249" s="10"/>
+      <c r="A249" s="16"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="A250" s="10"/>
+      <c r="A250" s="16"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="A251" s="10"/>
+      <c r="A251" s="16"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="A252" s="10"/>
+      <c r="A252" s="16"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="A253" s="10"/>
+      <c r="A253" s="16"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="A254" s="10"/>
+      <c r="A254" s="16"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="A255" s="10"/>
+      <c r="A255" s="16"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="A256" s="10"/>
+      <c r="A256" s="16"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="A257" s="10"/>
+      <c r="A257" s="16"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="A258" s="10"/>
+      <c r="A258" s="16"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="A259" s="10"/>
+      <c r="A259" s="16"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="A260" s="10"/>
+      <c r="A260" s="16"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="A261" s="10"/>
+      <c r="A261" s="16"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="A262" s="10"/>
+      <c r="A262" s="16"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="A263" s="10"/>
+      <c r="A263" s="16"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="A264" s="10"/>
+      <c r="A264" s="16"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="A265" s="10"/>
+      <c r="A265" s="16"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="A266" s="10"/>
+      <c r="A266" s="16"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="A267" s="10"/>
+      <c r="A267" s="16"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="A268" s="10"/>
+      <c r="A268" s="16"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="A269" s="10"/>
+      <c r="A269" s="16"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="A270" s="10"/>
+      <c r="A270" s="16"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="A271" s="10"/>
+      <c r="A271" s="16"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="A272" s="10"/>
+      <c r="A272" s="16"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="A273" s="10"/>
+      <c r="A273" s="16"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="A274" s="10"/>
+      <c r="A274" s="16"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="A275" s="10"/>
+      <c r="A275" s="16"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="A276" s="10"/>
+      <c r="A276" s="16"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="A277" s="10"/>
+      <c r="A277" s="16"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="A278" s="10"/>
+      <c r="A278" s="16"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="A279" s="10"/>
+      <c r="A279" s="16"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="A280" s="10"/>
+      <c r="A280" s="16"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="A281" s="10"/>
+      <c r="A281" s="16"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="A282" s="10"/>
+      <c r="A282" s="16"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="A283" s="10"/>
+      <c r="A283" s="16"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="A284" s="10"/>
+      <c r="A284" s="16"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="A285" s="10"/>
+      <c r="A285" s="16"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="A286" s="10"/>
+      <c r="A286" s="16"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="A287" s="10"/>
+      <c r="A287" s="16"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="A288" s="10"/>
+      <c r="A288" s="16"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="A289" s="10"/>
+      <c r="A289" s="16"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="A290" s="10"/>
+      <c r="A290" s="16"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="A291" s="10"/>
+      <c r="A291" s="16"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="A292" s="10"/>
+      <c r="A292" s="16"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="A293" s="10"/>
+      <c r="A293" s="16"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="A294" s="10"/>
+      <c r="A294" s="16"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="A295" s="10"/>
+      <c r="A295" s="16"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="A296" s="10"/>
+      <c r="A296" s="16"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="A297" s="10"/>
+      <c r="A297" s="16"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="A298" s="10"/>
+      <c r="A298" s="16"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="A299" s="10"/>
+      <c r="A299" s="16"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="A300" s="10"/>
+      <c r="A300" s="16"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="A301" s="10"/>
+      <c r="A301" s="16"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="A302" s="10"/>
+      <c r="A302" s="16"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="A303" s="10"/>
+      <c r="A303" s="16"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="A304" s="10"/>
+      <c r="A304" s="16"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="A305" s="10"/>
+      <c r="A305" s="16"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="A306" s="10"/>
+      <c r="A306" s="16"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="A307" s="10"/>
+      <c r="A307" s="16"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="A308" s="10"/>
+      <c r="A308" s="16"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="A309" s="10"/>
+      <c r="A309" s="16"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="A310" s="10"/>
+      <c r="A310" s="16"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="A311" s="10"/>
+      <c r="A311" s="16"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="A312" s="10"/>
+      <c r="A312" s="16"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="A313" s="10"/>
+      <c r="A313" s="16"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="A314" s="10"/>
+      <c r="A314" s="16"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
-      <c r="A315" s="10"/>
+      <c r="A315" s="16"/>
     </row>
     <row r="316" ht="15.75" customHeight="1">
-      <c r="A316" s="10"/>
+      <c r="A316" s="16"/>
     </row>
     <row r="317" ht="15.75" customHeight="1">
-      <c r="A317" s="10"/>
+      <c r="A317" s="16"/>
     </row>
     <row r="318" ht="15.75" customHeight="1">
-      <c r="A318" s="10"/>
+      <c r="A318" s="16"/>
     </row>
     <row r="319" ht="15.75" customHeight="1">
-      <c r="A319" s="10"/>
+      <c r="A319" s="16"/>
     </row>
     <row r="320" ht="15.75" customHeight="1">
-      <c r="A320" s="10"/>
+      <c r="A320" s="16"/>
     </row>
     <row r="321" ht="15.75" customHeight="1">
-      <c r="A321" s="10"/>
+      <c r="A321" s="16"/>
     </row>
     <row r="322" ht="15.75" customHeight="1">
-      <c r="A322" s="10"/>
+      <c r="A322" s="16"/>
     </row>
     <row r="323" ht="15.75" customHeight="1">
-      <c r="A323" s="10"/>
+      <c r="A323" s="16"/>
     </row>
     <row r="324" ht="15.75" customHeight="1">
-      <c r="A324" s="10"/>
+      <c r="A324" s="16"/>
     </row>
     <row r="325" ht="15.75" customHeight="1">
-      <c r="A325" s="10"/>
+      <c r="A325" s="16"/>
     </row>
     <row r="326" ht="15.75" customHeight="1">
-      <c r="A326" s="10"/>
+      <c r="A326" s="16"/>
     </row>
     <row r="327" ht="15.75" customHeight="1">
-      <c r="A327" s="10"/>
+      <c r="A327" s="16"/>
     </row>
     <row r="328" ht="15.75" customHeight="1">
-      <c r="A328" s="10"/>
+      <c r="A328" s="16"/>
     </row>
     <row r="329" ht="15.75" customHeight="1">
-      <c r="A329" s="10"/>
+      <c r="A329" s="16"/>
     </row>
     <row r="330" ht="15.75" customHeight="1">
-      <c r="A330" s="10"/>
+      <c r="A330" s="16"/>
     </row>
     <row r="331" ht="15.75" customHeight="1">
-      <c r="A331" s="10"/>
+      <c r="A331" s="16"/>
     </row>
     <row r="332" ht="15.75" customHeight="1">
-      <c r="A332" s="10"/>
+      <c r="A332" s="16"/>
     </row>
     <row r="333" ht="15.75" customHeight="1">
-      <c r="A333" s="10"/>
+      <c r="A333" s="16"/>
     </row>
     <row r="334" ht="15.75" customHeight="1">
-      <c r="A334" s="10"/>
+      <c r="A334" s="16"/>
     </row>
     <row r="335" ht="15.75" customHeight="1">
-      <c r="A335" s="10"/>
+      <c r="A335" s="16"/>
     </row>
     <row r="336" ht="15.75" customHeight="1">
-      <c r="A336" s="10"/>
+      <c r="A336" s="16"/>
     </row>
     <row r="337" ht="15.75" customHeight="1">
-      <c r="A337" s="10"/>
+      <c r="A337" s="16"/>
     </row>
     <row r="338" ht="15.75" customHeight="1">
-      <c r="A338" s="10"/>
+      <c r="A338" s="16"/>
     </row>
     <row r="339" ht="15.75" customHeight="1">
-      <c r="A339" s="10"/>
+      <c r="A339" s="16"/>
     </row>
     <row r="340" ht="15.75" customHeight="1">
-      <c r="A340" s="10"/>
+      <c r="A340" s="16"/>
     </row>
     <row r="341" ht="15.75" customHeight="1">
-      <c r="A341" s="10"/>
+      <c r="A341" s="16"/>
     </row>
     <row r="342" ht="15.75" customHeight="1">
-      <c r="A342" s="10"/>
+      <c r="A342" s="16"/>
     </row>
     <row r="343" ht="15.75" customHeight="1">
-      <c r="A343" s="10"/>
+      <c r="A343" s="16"/>
     </row>
     <row r="344" ht="15.75" customHeight="1">
-      <c r="A344" s="10"/>
+      <c r="A344" s="16"/>
     </row>
     <row r="345" ht="15.75" customHeight="1">
-      <c r="A345" s="10"/>
+      <c r="A345" s="16"/>
     </row>
     <row r="346" ht="15.75" customHeight="1">
-      <c r="A346" s="10"/>
+      <c r="A346" s="16"/>
     </row>
     <row r="347" ht="15.75" customHeight="1">
-      <c r="A347" s="10"/>
+      <c r="A347" s="16"/>
     </row>
     <row r="348" ht="15.75" customHeight="1">
-      <c r="A348" s="10"/>
+      <c r="A348" s="16"/>
     </row>
     <row r="349" ht="15.75" customHeight="1">
-      <c r="A349" s="10"/>
+      <c r="A349" s="16"/>
     </row>
     <row r="350" ht="15.75" customHeight="1">
-      <c r="A350" s="10"/>
+      <c r="A350" s="16"/>
     </row>
     <row r="351" ht="15.75" customHeight="1">
-      <c r="A351" s="10"/>
+      <c r="A351" s="16"/>
     </row>
     <row r="352" ht="15.75" customHeight="1">
-      <c r="A352" s="10"/>
+      <c r="A352" s="16"/>
     </row>
     <row r="353" ht="15.75" customHeight="1">
-      <c r="A353" s="10"/>
+      <c r="A353" s="16"/>
     </row>
     <row r="354" ht="15.75" customHeight="1">
-      <c r="A354" s="10"/>
+      <c r="A354" s="16"/>
     </row>
     <row r="355" ht="15.75" customHeight="1">
-      <c r="A355" s="10"/>
+      <c r="A355" s="16"/>
     </row>
     <row r="356" ht="15.75" customHeight="1">
-      <c r="A356" s="10"/>
+      <c r="A356" s="16"/>
     </row>
     <row r="357" ht="15.75" customHeight="1">
-      <c r="A357" s="10"/>
+      <c r="A357" s="16"/>
     </row>
     <row r="358" ht="15.75" customHeight="1">
-      <c r="A358" s="10"/>
+      <c r="A358" s="16"/>
     </row>
     <row r="359" ht="15.75" customHeight="1">
-      <c r="A359" s="10"/>
+      <c r="A359" s="16"/>
     </row>
     <row r="360" ht="15.75" customHeight="1">
-      <c r="A360" s="10"/>
+      <c r="A360" s="16"/>
     </row>
     <row r="361" ht="15.75" customHeight="1">
-      <c r="A361" s="10"/>
+      <c r="A361" s="16"/>
     </row>
     <row r="362" ht="15.75" customHeight="1">
-      <c r="A362" s="10"/>
+      <c r="A362" s="16"/>
     </row>
     <row r="363" ht="15.75" customHeight="1">
-      <c r="A363" s="10"/>
+      <c r="A363" s="16"/>
     </row>
     <row r="364" ht="15.75" customHeight="1">
-      <c r="A364" s="10"/>
+      <c r="A364" s="16"/>
     </row>
     <row r="365" ht="15.75" customHeight="1">
-      <c r="A365" s="10"/>
+      <c r="A365" s="16"/>
     </row>
     <row r="366" ht="15.75" customHeight="1">
-      <c r="A366" s="10"/>
+      <c r="A366" s="16"/>
     </row>
     <row r="367" ht="15.75" customHeight="1">
-      <c r="A367" s="10"/>
+      <c r="A367" s="16"/>
     </row>
     <row r="368" ht="15.75" customHeight="1">
-      <c r="A368" s="10"/>
+      <c r="A368" s="16"/>
     </row>
     <row r="369" ht="15.75" customHeight="1">
-      <c r="A369" s="10"/>
+      <c r="A369" s="16"/>
     </row>
     <row r="370" ht="15.75" customHeight="1">
-      <c r="A370" s="10"/>
+      <c r="A370" s="16"/>
     </row>
     <row r="371" ht="15.75" customHeight="1">
-      <c r="A371" s="10"/>
+      <c r="A371" s="16"/>
     </row>
     <row r="372" ht="15.75" customHeight="1">
-      <c r="A372" s="10"/>
+      <c r="A372" s="16"/>
     </row>
     <row r="373" ht="15.75" customHeight="1">
-      <c r="A373" s="10"/>
+      <c r="A373" s="16"/>
     </row>
     <row r="374" ht="15.75" customHeight="1">
-      <c r="A374" s="10"/>
+      <c r="A374" s="16"/>
     </row>
     <row r="375" ht="15.75" customHeight="1">
-      <c r="A375" s="10"/>
+      <c r="A375" s="16"/>
     </row>
     <row r="376" ht="15.75" customHeight="1">
-      <c r="A376" s="10"/>
+      <c r="A376" s="16"/>
     </row>
     <row r="377" ht="15.75" customHeight="1">
-      <c r="A377" s="10"/>
+      <c r="A377" s="16"/>
     </row>
     <row r="378" ht="15.75" customHeight="1">
-      <c r="A378" s="10"/>
+      <c r="A378" s="16"/>
     </row>
     <row r="379" ht="15.75" customHeight="1">
-      <c r="A379" s="10"/>
+      <c r="A379" s="16"/>
     </row>
     <row r="380" ht="15.75" customHeight="1">
-      <c r="A380" s="10"/>
+      <c r="A380" s="16"/>
     </row>
     <row r="381" ht="15.75" customHeight="1">
-      <c r="A381" s="10"/>
+      <c r="A381" s="16"/>
     </row>
     <row r="382" ht="15.75" customHeight="1">
-      <c r="A382" s="10"/>
+      <c r="A382" s="16"/>
     </row>
     <row r="383" ht="15.75" customHeight="1">
-      <c r="A383" s="10"/>
+      <c r="A383" s="16"/>
     </row>
     <row r="384" ht="15.75" customHeight="1">
-      <c r="A384" s="10"/>
+      <c r="A384" s="16"/>
     </row>
     <row r="385" ht="15.75" customHeight="1">
-      <c r="A385" s="10"/>
+      <c r="A385" s="16"/>
     </row>
     <row r="386" ht="15.75" customHeight="1">
-      <c r="A386" s="10"/>
+      <c r="A386" s="16"/>
     </row>
     <row r="387" ht="15.75" customHeight="1">
-      <c r="A387" s="10"/>
+      <c r="A387" s="16"/>
     </row>
     <row r="388" ht="15.75" customHeight="1">
-      <c r="A388" s="10"/>
+      <c r="A388" s="16"/>
     </row>
     <row r="389" ht="15.75" customHeight="1">
-      <c r="A389" s="10"/>
+      <c r="A389" s="16"/>
     </row>
     <row r="390" ht="15.75" customHeight="1">
-      <c r="A390" s="10"/>
+      <c r="A390" s="16"/>
     </row>
     <row r="391" ht="15.75" customHeight="1">
-      <c r="A391" s="10"/>
+      <c r="A391" s="16"/>
     </row>
     <row r="392" ht="15.75" customHeight="1">
-      <c r="A392" s="10"/>
+      <c r="A392" s="16"/>
     </row>
     <row r="393" ht="15.75" customHeight="1">
-      <c r="A393" s="10"/>
+      <c r="A393" s="16"/>
     </row>
     <row r="394" ht="15.75" customHeight="1">
-      <c r="A394" s="10"/>
+      <c r="A394" s="16"/>
     </row>
     <row r="395" ht="15.75" customHeight="1">
-      <c r="A395" s="10"/>
+      <c r="A395" s="16"/>
     </row>
     <row r="396" ht="15.75" customHeight="1">
-      <c r="A396" s="10"/>
+      <c r="A396" s="16"/>
     </row>
     <row r="397" ht="15.75" customHeight="1">
-      <c r="A397" s="10"/>
+      <c r="A397" s="16"/>
     </row>
     <row r="398" ht="15.75" customHeight="1">
-      <c r="A398" s="10"/>
+      <c r="A398" s="16"/>
     </row>
     <row r="399" ht="15.75" customHeight="1">
-      <c r="A399" s="10"/>
+      <c r="A399" s="16"/>
     </row>
     <row r="400" ht="15.75" customHeight="1">
-      <c r="A400" s="10"/>
+      <c r="A400" s="16"/>
     </row>
     <row r="401" ht="15.75" customHeight="1">
-      <c r="A401" s="10"/>
+      <c r="A401" s="16"/>
     </row>
     <row r="402" ht="15.75" customHeight="1">
-      <c r="A402" s="10"/>
+      <c r="A402" s="16"/>
     </row>
     <row r="403" ht="15.75" customHeight="1">
-      <c r="A403" s="10"/>
+      <c r="A403" s="16"/>
     </row>
     <row r="404" ht="15.75" customHeight="1">
-      <c r="A404" s="10"/>
+      <c r="A404" s="16"/>
     </row>
     <row r="405" ht="15.75" customHeight="1">
-      <c r="A405" s="10"/>
+      <c r="A405" s="16"/>
     </row>
     <row r="406" ht="15.75" customHeight="1">
-      <c r="A406" s="10"/>
+      <c r="A406" s="16"/>
     </row>
     <row r="407" ht="15.75" customHeight="1">
-      <c r="A407" s="10"/>
+      <c r="A407" s="16"/>
     </row>
     <row r="408" ht="15.75" customHeight="1">
-      <c r="A408" s="10"/>
+      <c r="A408" s="16"/>
     </row>
     <row r="409" ht="15.75" customHeight="1">
-      <c r="A409" s="10"/>
+      <c r="A409" s="16"/>
     </row>
     <row r="410" ht="15.75" customHeight="1">
-      <c r="A410" s="10"/>
+      <c r="A410" s="16"/>
     </row>
     <row r="411" ht="15.75" customHeight="1">
-      <c r="A411" s="10"/>
+      <c r="A411" s="16"/>
     </row>
     <row r="412" ht="15.75" customHeight="1">
-      <c r="A412" s="10"/>
+      <c r="A412" s="16"/>
     </row>
     <row r="413" ht="15.75" customHeight="1">
-      <c r="A413" s="10"/>
+      <c r="A413" s="16"/>
     </row>
     <row r="414" ht="15.75" customHeight="1">
-      <c r="A414" s="10"/>
+      <c r="A414" s="16"/>
     </row>
     <row r="415" ht="15.75" customHeight="1">
-      <c r="A415" s="10"/>
+      <c r="A415" s="16"/>
     </row>
     <row r="416" ht="15.75" customHeight="1">
-      <c r="A416" s="10"/>
+      <c r="A416" s="16"/>
     </row>
     <row r="417" ht="15.75" customHeight="1">
-      <c r="A417" s="10"/>
+      <c r="A417" s="16"/>
     </row>
     <row r="418" ht="15.75" customHeight="1">
-      <c r="A418" s="10"/>
+      <c r="A418" s="16"/>
     </row>
     <row r="419" ht="15.75" customHeight="1">
-      <c r="A419" s="10"/>
+      <c r="A419" s="16"/>
     </row>
     <row r="420" ht="15.75" customHeight="1">
-      <c r="A420" s="10"/>
+      <c r="A420" s="16"/>
     </row>
     <row r="421" ht="15.75" customHeight="1">
-      <c r="A421" s="10"/>
+      <c r="A421" s="16"/>
     </row>
     <row r="422" ht="15.75" customHeight="1">
-      <c r="A422" s="10"/>
+      <c r="A422" s="16"/>
     </row>
     <row r="423" ht="15.75" customHeight="1">
-      <c r="A423" s="10"/>
+      <c r="A423" s="16"/>
     </row>
     <row r="424" ht="15.75" customHeight="1">
-      <c r="A424" s="10"/>
+      <c r="A424" s="16"/>
     </row>
     <row r="425" ht="15.75" customHeight="1">
-      <c r="A425" s="10"/>
+      <c r="A425" s="16"/>
     </row>
     <row r="426" ht="15.75" customHeight="1">
-      <c r="A426" s="10"/>
+      <c r="A426" s="16"/>
     </row>
     <row r="427" ht="15.75" customHeight="1">
-      <c r="A427" s="10"/>
+      <c r="A427" s="16"/>
     </row>
     <row r="428" ht="15.75" customHeight="1">
-      <c r="A428" s="10"/>
+      <c r="A428" s="16"/>
     </row>
     <row r="429" ht="15.75" customHeight="1">
-      <c r="A429" s="10"/>
+      <c r="A429" s="16"/>
     </row>
     <row r="430" ht="15.75" customHeight="1">
-      <c r="A430" s="10"/>
+      <c r="A430" s="16"/>
     </row>
     <row r="431" ht="15.75" customHeight="1">
-      <c r="A431" s="10"/>
+      <c r="A431" s="16"/>
     </row>
     <row r="432" ht="15.75" customHeight="1">
-      <c r="A432" s="10"/>
+      <c r="A432" s="16"/>
     </row>
     <row r="433" ht="15.75" customHeight="1">
-      <c r="A433" s="10"/>
+      <c r="A433" s="16"/>
     </row>
     <row r="434" ht="15.75" customHeight="1">
-      <c r="A434" s="10"/>
+      <c r="A434" s="16"/>
     </row>
     <row r="435" ht="15.75" customHeight="1">
-      <c r="A435" s="10"/>
+      <c r="A435" s="16"/>
     </row>
     <row r="436" ht="15.75" customHeight="1">
-      <c r="A436" s="10"/>
+      <c r="A436" s="16"/>
     </row>
     <row r="437" ht="15.75" customHeight="1">
-      <c r="A437" s="10"/>
+      <c r="A437" s="16"/>
     </row>
     <row r="438" ht="15.75" customHeight="1">
-      <c r="A438" s="10"/>
+      <c r="A438" s="16"/>
     </row>
     <row r="439" ht="15.75" customHeight="1">
-      <c r="A439" s="10"/>
+      <c r="A439" s="16"/>
     </row>
     <row r="440" ht="15.75" customHeight="1">
-      <c r="A440" s="10"/>
+      <c r="A440" s="16"/>
     </row>
     <row r="441" ht="15.75" customHeight="1">
-      <c r="A441" s="10"/>
+      <c r="A441" s="16"/>
     </row>
     <row r="442" ht="15.75" customHeight="1">
-      <c r="A442" s="10"/>
+      <c r="A442" s="16"/>
     </row>
     <row r="443" ht="15.75" customHeight="1">
-      <c r="A443" s="10"/>
+      <c r="A443" s="16"/>
     </row>
     <row r="444" ht="15.75" customHeight="1">
-      <c r="A444" s="10"/>
+      <c r="A444" s="16"/>
     </row>
     <row r="445" ht="15.75" customHeight="1">
-      <c r="A445" s="10"/>
+      <c r="A445" s="16"/>
     </row>
     <row r="446" ht="15.75" customHeight="1">
-      <c r="A446" s="10"/>
+      <c r="A446" s="16"/>
     </row>
     <row r="447" ht="15.75" customHeight="1">
-      <c r="A447" s="10"/>
+      <c r="A447" s="16"/>
     </row>
     <row r="448" ht="15.75" customHeight="1">
-      <c r="A448" s="10"/>
+      <c r="A448" s="16"/>
     </row>
     <row r="449" ht="15.75" customHeight="1">
-      <c r="A449" s="10"/>
+      <c r="A449" s="16"/>
     </row>
     <row r="450" ht="15.75" customHeight="1">
-      <c r="A450" s="10"/>
+      <c r="A450" s="16"/>
     </row>
     <row r="451" ht="15.75" customHeight="1">
-      <c r="A451" s="10"/>
+      <c r="A451" s="16"/>
     </row>
     <row r="452" ht="15.75" customHeight="1">
-      <c r="A452" s="10"/>
+      <c r="A452" s="16"/>
     </row>
     <row r="453" ht="15.75" customHeight="1">
-      <c r="A453" s="10"/>
+      <c r="A453" s="16"/>
     </row>
     <row r="454" ht="15.75" customHeight="1">
-      <c r="A454" s="10"/>
+      <c r="A454" s="16"/>
     </row>
     <row r="455" ht="15.75" customHeight="1">
-      <c r="A455" s="10"/>
+      <c r="A455" s="16"/>
     </row>
     <row r="456" ht="15.75" customHeight="1">
-      <c r="A456" s="10"/>
+      <c r="A456" s="16"/>
     </row>
     <row r="457" ht="15.75" customHeight="1">
-      <c r="A457" s="10"/>
+      <c r="A457" s="16"/>
     </row>
     <row r="458" ht="15.75" customHeight="1">
-      <c r="A458" s="10"/>
+      <c r="A458" s="16"/>
     </row>
     <row r="459" ht="15.75" customHeight="1">
-      <c r="A459" s="10"/>
+      <c r="A459" s="16"/>
     </row>
     <row r="460" ht="15.75" customHeight="1">
-      <c r="A460" s="10"/>
+      <c r="A460" s="16"/>
     </row>
     <row r="461" ht="15.75" customHeight="1">
-      <c r="A461" s="10"/>
+      <c r="A461" s="16"/>
     </row>
     <row r="462" ht="15.75" customHeight="1">
-      <c r="A462" s="10"/>
+      <c r="A462" s="16"/>
     </row>
     <row r="463" ht="15.75" customHeight="1">
-      <c r="A463" s="10"/>
+      <c r="A463" s="16"/>
     </row>
     <row r="464" ht="15.75" customHeight="1">
-      <c r="A464" s="10"/>
+      <c r="A464" s="16"/>
     </row>
     <row r="465" ht="15.75" customHeight="1">
-      <c r="A465" s="10"/>
+      <c r="A465" s="16"/>
     </row>
     <row r="466" ht="15.75" customHeight="1">
-      <c r="A466" s="10"/>
+      <c r="A466" s="16"/>
     </row>
     <row r="467" ht="15.75" customHeight="1">
-      <c r="A467" s="10"/>
+      <c r="A467" s="16"/>
     </row>
     <row r="468" ht="15.75" customHeight="1">
-      <c r="A468" s="10"/>
+      <c r="A468" s="16"/>
     </row>
     <row r="469" ht="15.75" customHeight="1">
-      <c r="A469" s="10"/>
+      <c r="A469" s="16"/>
     </row>
     <row r="470" ht="15.75" customHeight="1">
-      <c r="A470" s="10"/>
+      <c r="A470" s="16"/>
     </row>
     <row r="471" ht="15.75" customHeight="1">
-      <c r="A471" s="10"/>
+      <c r="A471" s="16"/>
     </row>
     <row r="472" ht="15.75" customHeight="1">
-      <c r="A472" s="10"/>
+      <c r="A472" s="16"/>
     </row>
     <row r="473" ht="15.75" customHeight="1">
-      <c r="A473" s="10"/>
+      <c r="A473" s="16"/>
     </row>
     <row r="474" ht="15.75" customHeight="1">
-      <c r="A474" s="10"/>
+      <c r="A474" s="16"/>
     </row>
     <row r="475" ht="15.75" customHeight="1">
-      <c r="A475" s="10"/>
+      <c r="A475" s="16"/>
     </row>
     <row r="476" ht="15.75" customHeight="1">
-      <c r="A476" s="10"/>
+      <c r="A476" s="16"/>
     </row>
     <row r="477" ht="15.75" customHeight="1">
-      <c r="A477" s="10"/>
+      <c r="A477" s="16"/>
     </row>
     <row r="478" ht="15.75" customHeight="1">
-      <c r="A478" s="10"/>
+      <c r="A478" s="16"/>
     </row>
     <row r="479" ht="15.75" customHeight="1">
-      <c r="A479" s="10"/>
+      <c r="A479" s="16"/>
     </row>
     <row r="480" ht="15.75" customHeight="1">
-      <c r="A480" s="10"/>
+      <c r="A480" s="16"/>
     </row>
     <row r="481" ht="15.75" customHeight="1">
-      <c r="A481" s="10"/>
+      <c r="A481" s="16"/>
     </row>
     <row r="482" ht="15.75" customHeight="1">
-      <c r="A482" s="10"/>
+      <c r="A482" s="16"/>
     </row>
     <row r="483" ht="15.75" customHeight="1">
-      <c r="A483" s="10"/>
+      <c r="A483" s="16"/>
     </row>
     <row r="484" ht="15.75" customHeight="1">
-      <c r="A484" s="10"/>
+      <c r="A484" s="16"/>
     </row>
     <row r="485" ht="15.75" customHeight="1">
-      <c r="A485" s="10"/>
+      <c r="A485" s="16"/>
     </row>
     <row r="486" ht="15.75" customHeight="1">
-      <c r="A486" s="10"/>
+      <c r="A486" s="16"/>
     </row>
     <row r="487" ht="15.75" customHeight="1">
-      <c r="A487" s="10"/>
+      <c r="A487" s="16"/>
     </row>
     <row r="488" ht="15.75" customHeight="1">
-      <c r="A488" s="10"/>
+      <c r="A488" s="16"/>
     </row>
     <row r="489" ht="15.75" customHeight="1">
-      <c r="A489" s="10"/>
+      <c r="A489" s="16"/>
     </row>
     <row r="490" ht="15.75" customHeight="1">
-      <c r="A490" s="10"/>
+      <c r="A490" s="16"/>
     </row>
     <row r="491" ht="15.75" customHeight="1">
-      <c r="A491" s="10"/>
+      <c r="A491" s="16"/>
     </row>
     <row r="492" ht="15.75" customHeight="1">
-      <c r="A492" s="10"/>
+      <c r="A492" s="16"/>
     </row>
     <row r="493" ht="15.75" customHeight="1">
-      <c r="A493" s="10"/>
+      <c r="A493" s="16"/>
     </row>
     <row r="494" ht="15.75" customHeight="1">
-      <c r="A494" s="10"/>
+      <c r="A494" s="16"/>
     </row>
     <row r="495" ht="15.75" customHeight="1">
-      <c r="A495" s="10"/>
+      <c r="A495" s="16"/>
     </row>
     <row r="496" ht="15.75" customHeight="1">
-      <c r="A496" s="10"/>
+      <c r="A496" s="16"/>
     </row>
     <row r="497" ht="15.75" customHeight="1">
-      <c r="A497" s="10"/>
+      <c r="A497" s="16"/>
     </row>
     <row r="498" ht="15.75" customHeight="1">
-      <c r="A498" s="10"/>
+      <c r="A498" s="16"/>
     </row>
     <row r="499" ht="15.75" customHeight="1">
-      <c r="A499" s="10"/>
+      <c r="A499" s="16"/>
     </row>
     <row r="500" ht="15.75" customHeight="1">
-      <c r="A500" s="10"/>
+      <c r="A500" s="16"/>
     </row>
     <row r="501" ht="15.75" customHeight="1">
-      <c r="A501" s="10"/>
+      <c r="A501" s="16"/>
     </row>
     <row r="502" ht="15.75" customHeight="1">
-      <c r="A502" s="10"/>
+      <c r="A502" s="16"/>
     </row>
     <row r="503" ht="15.75" customHeight="1">
-      <c r="A503" s="10"/>
+      <c r="A503" s="16"/>
     </row>
     <row r="504" ht="15.75" customHeight="1">
-      <c r="A504" s="10"/>
+      <c r="A504" s="16"/>
     </row>
     <row r="505" ht="15.75" customHeight="1">
-      <c r="A505" s="10"/>
+      <c r="A505" s="16"/>
     </row>
     <row r="506" ht="15.75" customHeight="1">
-      <c r="A506" s="10"/>
+      <c r="A506" s="16"/>
     </row>
     <row r="507" ht="15.75" customHeight="1">
-      <c r="A507" s="10"/>
+      <c r="A507" s="16"/>
     </row>
     <row r="508" ht="15.75" customHeight="1">
-      <c r="A508" s="10"/>
+      <c r="A508" s="16"/>
     </row>
     <row r="509" ht="15.75" customHeight="1">
-      <c r="A509" s="10"/>
+      <c r="A509" s="16"/>
     </row>
     <row r="510" ht="15.75" customHeight="1">
-      <c r="A510" s="10"/>
+      <c r="A510" s="16"/>
     </row>
     <row r="511" ht="15.75" customHeight="1">
-      <c r="A511" s="10"/>
+      <c r="A511" s="16"/>
     </row>
     <row r="512" ht="15.75" customHeight="1">
-      <c r="A512" s="10"/>
+      <c r="A512" s="16"/>
     </row>
     <row r="513" ht="15.75" customHeight="1">
-      <c r="A513" s="10"/>
+      <c r="A513" s="16"/>
     </row>
     <row r="514" ht="15.75" customHeight="1">
-      <c r="A514" s="10"/>
+      <c r="A514" s="16"/>
     </row>
     <row r="515" ht="15.75" customHeight="1">
-      <c r="A515" s="10"/>
+      <c r="A515" s="16"/>
     </row>
     <row r="516" ht="15.75" customHeight="1">
-      <c r="A516" s="10"/>
+      <c r="A516" s="16"/>
     </row>
     <row r="517" ht="15.75" customHeight="1">
-      <c r="A517" s="10"/>
+      <c r="A517" s="16"/>
     </row>
     <row r="518" ht="15.75" customHeight="1">
-      <c r="A518" s="10"/>
+      <c r="A518" s="16"/>
     </row>
     <row r="519" ht="15.75" customHeight="1">
-      <c r="A519" s="10"/>
+      <c r="A519" s="16"/>
     </row>
     <row r="520" ht="15.75" customHeight="1">
-      <c r="A520" s="10"/>
+      <c r="A520" s="16"/>
     </row>
     <row r="521" ht="15.75" customHeight="1">
-      <c r="A521" s="10"/>
+      <c r="A521" s="16"/>
     </row>
     <row r="522" ht="15.75" customHeight="1">
-      <c r="A522" s="10"/>
+      <c r="A522" s="16"/>
     </row>
     <row r="523" ht="15.75" customHeight="1">
-      <c r="A523" s="10"/>
+      <c r="A523" s="16"/>
     </row>
     <row r="524" ht="15.75" customHeight="1">
-      <c r="A524" s="10"/>
+      <c r="A524" s="16"/>
     </row>
     <row r="525" ht="15.75" customHeight="1">
-      <c r="A525" s="10"/>
+      <c r="A525" s="16"/>
     </row>
     <row r="526" ht="15.75" customHeight="1">
-      <c r="A526" s="10"/>
+      <c r="A526" s="16"/>
     </row>
     <row r="527" ht="15.75" customHeight="1">
-      <c r="A527" s="10"/>
+      <c r="A527" s="16"/>
     </row>
     <row r="528" ht="15.75" customHeight="1">
-      <c r="A528" s="10"/>
+      <c r="A528" s="16"/>
     </row>
     <row r="529" ht="15.75" customHeight="1">
-      <c r="A529" s="10"/>
+      <c r="A529" s="16"/>
     </row>
     <row r="530" ht="15.75" customHeight="1">
-      <c r="A530" s="10"/>
+      <c r="A530" s="16"/>
     </row>
     <row r="531" ht="15.75" customHeight="1">
-      <c r="A531" s="10"/>
+      <c r="A531" s="16"/>
     </row>
     <row r="532" ht="15.75" customHeight="1">
-      <c r="A532" s="10"/>
+      <c r="A532" s="16"/>
     </row>
     <row r="533" ht="15.75" customHeight="1">
-      <c r="A533" s="10"/>
+      <c r="A533" s="16"/>
     </row>
     <row r="534" ht="15.75" customHeight="1">
-      <c r="A534" s="10"/>
+      <c r="A534" s="16"/>
     </row>
     <row r="535" ht="15.75" customHeight="1">
-      <c r="A535" s="10"/>
+      <c r="A535" s="16"/>
     </row>
     <row r="536" ht="15.75" customHeight="1">
-      <c r="A536" s="10"/>
+      <c r="A536" s="16"/>
     </row>
     <row r="537" ht="15.75" customHeight="1">
-      <c r="A537" s="10"/>
+      <c r="A537" s="16"/>
     </row>
     <row r="538" ht="15.75" customHeight="1">
-      <c r="A538" s="10"/>
+      <c r="A538" s="16"/>
     </row>
     <row r="539" ht="15.75" customHeight="1">
-      <c r="A539" s="10"/>
+      <c r="A539" s="16"/>
     </row>
     <row r="540" ht="15.75" customHeight="1">
-      <c r="A540" s="10"/>
+      <c r="A540" s="16"/>
     </row>
     <row r="541" ht="15.75" customHeight="1">
-      <c r="A541" s="10"/>
+      <c r="A541" s="16"/>
     </row>
     <row r="542" ht="15.75" customHeight="1">
-      <c r="A542" s="10"/>
+      <c r="A542" s="16"/>
     </row>
     <row r="543" ht="15.75" customHeight="1">
-      <c r="A543" s="10"/>
+      <c r="A543" s="16"/>
     </row>
     <row r="544" ht="15.75" customHeight="1">
-      <c r="A544" s="10"/>
+      <c r="A544" s="16"/>
     </row>
     <row r="545" ht="15.75" customHeight="1">
-      <c r="A545" s="10"/>
+      <c r="A545" s="16"/>
     </row>
     <row r="546" ht="15.75" customHeight="1">
-      <c r="A546" s="10"/>
+      <c r="A546" s="16"/>
     </row>
     <row r="547" ht="15.75" customHeight="1">
-      <c r="A547" s="10"/>
+      <c r="A547" s="16"/>
     </row>
     <row r="548" ht="15.75" customHeight="1">
-      <c r="A548" s="10"/>
+      <c r="A548" s="16"/>
     </row>
     <row r="549" ht="15.75" customHeight="1">
-      <c r="A549" s="10"/>
+      <c r="A549" s="16"/>
     </row>
     <row r="550" ht="15.75" customHeight="1">
-      <c r="A550" s="10"/>
+      <c r="A550" s="16"/>
     </row>
     <row r="551" ht="15.75" customHeight="1">
-      <c r="A551" s="10"/>
+      <c r="A551" s="16"/>
     </row>
     <row r="552" ht="15.75" customHeight="1">
-      <c r="A552" s="10"/>
+      <c r="A552" s="16"/>
     </row>
     <row r="553" ht="15.75" customHeight="1">
-      <c r="A553" s="10"/>
+      <c r="A553" s="16"/>
     </row>
     <row r="554" ht="15.75" customHeight="1">
-      <c r="A554" s="10"/>
+      <c r="A554" s="16"/>
     </row>
     <row r="555" ht="15.75" customHeight="1">
-      <c r="A555" s="10"/>
+      <c r="A555" s="16"/>
     </row>
     <row r="556" ht="15.75" customHeight="1">
-      <c r="A556" s="10"/>
+      <c r="A556" s="16"/>
     </row>
     <row r="557" ht="15.75" customHeight="1">
-      <c r="A557" s="10"/>
+      <c r="A557" s="16"/>
     </row>
     <row r="558" ht="15.75" customHeight="1">
-      <c r="A558" s="10"/>
+      <c r="A558" s="16"/>
     </row>
     <row r="559" ht="15.75" customHeight="1">
-      <c r="A559" s="10"/>
+      <c r="A559" s="16"/>
     </row>
     <row r="560" ht="15.75" customHeight="1">
-      <c r="A560" s="10"/>
+      <c r="A560" s="16"/>
     </row>
     <row r="561" ht="15.75" customHeight="1">
-      <c r="A561" s="10"/>
+      <c r="A561" s="16"/>
     </row>
     <row r="562" ht="15.75" customHeight="1">
-      <c r="A562" s="10"/>
+      <c r="A562" s="16"/>
     </row>
     <row r="563" ht="15.75" customHeight="1">
-      <c r="A563" s="10"/>
+      <c r="A563" s="16"/>
     </row>
     <row r="564" ht="15.75" customHeight="1">
-      <c r="A564" s="10"/>
+      <c r="A564" s="16"/>
     </row>
     <row r="565" ht="15.75" customHeight="1">
-      <c r="A565" s="10"/>
+      <c r="A565" s="16"/>
     </row>
     <row r="566" ht="15.75" customHeight="1">
-      <c r="A566" s="10"/>
+      <c r="A566" s="16"/>
     </row>
     <row r="567" ht="15.75" customHeight="1">
-      <c r="A567" s="10"/>
+      <c r="A567" s="16"/>
     </row>
     <row r="568" ht="15.75" customHeight="1">
-      <c r="A568" s="10"/>
+      <c r="A568" s="16"/>
     </row>
     <row r="569" ht="15.75" customHeight="1">
-      <c r="A569" s="10"/>
+      <c r="A569" s="16"/>
     </row>
     <row r="570" ht="15.75" customHeight="1">
-      <c r="A570" s="10"/>
+      <c r="A570" s="16"/>
     </row>
     <row r="571" ht="15.75" customHeight="1">
-      <c r="A571" s="10"/>
+      <c r="A571" s="16"/>
     </row>
     <row r="572" ht="15.75" customHeight="1">
-      <c r="A572" s="10"/>
+      <c r="A572" s="16"/>
     </row>
     <row r="573" ht="15.75" customHeight="1">
-      <c r="A573" s="10"/>
+      <c r="A573" s="16"/>
     </row>
     <row r="574" ht="15.75" customHeight="1">
-      <c r="A574" s="10"/>
+      <c r="A574" s="16"/>
     </row>
     <row r="575" ht="15.75" customHeight="1">
-      <c r="A575" s="10"/>
+      <c r="A575" s="16"/>
     </row>
     <row r="576" ht="15.75" customHeight="1">
-      <c r="A576" s="10"/>
+      <c r="A576" s="16"/>
     </row>
     <row r="577" ht="15.75" customHeight="1">
-      <c r="A577" s="10"/>
+      <c r="A577" s="16"/>
     </row>
     <row r="578" ht="15.75" customHeight="1">
-      <c r="A578" s="10"/>
+      <c r="A578" s="16"/>
     </row>
     <row r="579" ht="15.75" customHeight="1">
-      <c r="A579" s="10"/>
+      <c r="A579" s="16"/>
     </row>
     <row r="580" ht="15.75" customHeight="1">
-      <c r="A580" s="10"/>
+      <c r="A580" s="16"/>
     </row>
     <row r="581" ht="15.75" customHeight="1">
-      <c r="A581" s="10"/>
+      <c r="A581" s="16"/>
     </row>
     <row r="582" ht="15.75" customHeight="1">
-      <c r="A582" s="10"/>
+      <c r="A582" s="16"/>
     </row>
     <row r="583" ht="15.75" customHeight="1">
-      <c r="A583" s="10"/>
+      <c r="A583" s="16"/>
     </row>
     <row r="584" ht="15.75" customHeight="1">
-      <c r="A584" s="10"/>
+      <c r="A584" s="16"/>
     </row>
     <row r="585" ht="15.75" customHeight="1">
-      <c r="A585" s="10"/>
+      <c r="A585" s="16"/>
     </row>
     <row r="586" ht="15.75" customHeight="1">
-      <c r="A586" s="10"/>
+      <c r="A586" s="16"/>
     </row>
     <row r="587" ht="15.75" customHeight="1">
-      <c r="A587" s="10"/>
+      <c r="A587" s="16"/>
     </row>
     <row r="588" ht="15.75" customHeight="1">
-      <c r="A588" s="10"/>
+      <c r="A588" s="16"/>
     </row>
     <row r="589" ht="15.75" customHeight="1">
-      <c r="A589" s="10"/>
+      <c r="A589" s="16"/>
     </row>
     <row r="590" ht="15.75" customHeight="1">
-      <c r="A590" s="10"/>
+      <c r="A590" s="16"/>
     </row>
     <row r="591" ht="15.75" customHeight="1">
-      <c r="A591" s="10"/>
+      <c r="A591" s="16"/>
     </row>
     <row r="592" ht="15.75" customHeight="1">
-      <c r="A592" s="10"/>
+      <c r="A592" s="16"/>
     </row>
     <row r="593" ht="15.75" customHeight="1">
-      <c r="A593" s="10"/>
+      <c r="A593" s="16"/>
     </row>
     <row r="594" ht="15.75" customHeight="1">
-      <c r="A594" s="10"/>
+      <c r="A594" s="16"/>
     </row>
     <row r="595" ht="15.75" customHeight="1">
-      <c r="A595" s="10"/>
+      <c r="A595" s="16"/>
     </row>
     <row r="596" ht="15.75" customHeight="1">
-      <c r="A596" s="10"/>
+      <c r="A596" s="16"/>
     </row>
     <row r="597" ht="15.75" customHeight="1">
-      <c r="A597" s="10"/>
+      <c r="A597" s="16"/>
     </row>
     <row r="598" ht="15.75" customHeight="1">
-      <c r="A598" s="10"/>
+      <c r="A598" s="16"/>
     </row>
     <row r="599" ht="15.75" customHeight="1">
-      <c r="A599" s="10"/>
+      <c r="A599" s="16"/>
     </row>
     <row r="600" ht="15.75" customHeight="1">
-      <c r="A600" s="10"/>
+      <c r="A600" s="16"/>
     </row>
     <row r="601" ht="15.75" customHeight="1">
-      <c r="A601" s="10"/>
+      <c r="A601" s="16"/>
     </row>
     <row r="602" ht="15.75" customHeight="1">
-      <c r="A602" s="10"/>
+      <c r="A602" s="16"/>
     </row>
     <row r="603" ht="15.75" customHeight="1">
-      <c r="A603" s="10"/>
+      <c r="A603" s="16"/>
     </row>
     <row r="604" ht="15.75" customHeight="1">
-      <c r="A604" s="10"/>
+      <c r="A604" s="16"/>
     </row>
     <row r="605" ht="15.75" customHeight="1">
-      <c r="A605" s="10"/>
+      <c r="A605" s="16"/>
     </row>
     <row r="606" ht="15.75" customHeight="1">
-      <c r="A606" s="10"/>
+      <c r="A606" s="16"/>
     </row>
     <row r="607" ht="15.75" customHeight="1">
-      <c r="A607" s="10"/>
+      <c r="A607" s="16"/>
     </row>
     <row r="608" ht="15.75" customHeight="1">
-      <c r="A608" s="10"/>
+      <c r="A608" s="16"/>
     </row>
     <row r="609" ht="15.75" customHeight="1">
-      <c r="A609" s="10"/>
+      <c r="A609" s="16"/>
     </row>
     <row r="610" ht="15.75" customHeight="1">
-      <c r="A610" s="10"/>
+      <c r="A610" s="16"/>
     </row>
     <row r="611" ht="15.75" customHeight="1">
-      <c r="A611" s="10"/>
+      <c r="A611" s="16"/>
     </row>
     <row r="612" ht="15.75" customHeight="1">
-      <c r="A612" s="10"/>
+      <c r="A612" s="16"/>
     </row>
     <row r="613" ht="15.75" customHeight="1">
-      <c r="A613" s="10"/>
+      <c r="A613" s="16"/>
     </row>
     <row r="614" ht="15.75" customHeight="1">
-      <c r="A614" s="10"/>
+      <c r="A614" s="16"/>
     </row>
     <row r="615" ht="15.75" customHeight="1">
-      <c r="A615" s="10"/>
+      <c r="A615" s="16"/>
     </row>
     <row r="616" ht="15.75" customHeight="1">
-      <c r="A616" s="10"/>
+      <c r="A616" s="16"/>
     </row>
     <row r="617" ht="15.75" customHeight="1">
-      <c r="A617" s="10"/>
+      <c r="A617" s="16"/>
     </row>
     <row r="618" ht="15.75" customHeight="1">
-      <c r="A618" s="10"/>
+      <c r="A618" s="16"/>
     </row>
     <row r="619" ht="15.75" customHeight="1">
-      <c r="A619" s="10"/>
+      <c r="A619" s="16"/>
     </row>
     <row r="620" ht="15.75" customHeight="1">
-      <c r="A620" s="10"/>
+      <c r="A620" s="16"/>
     </row>
     <row r="621" ht="15.75" customHeight="1">
-      <c r="A621" s="10"/>
+      <c r="A621" s="16"/>
     </row>
     <row r="622" ht="15.75" customHeight="1">
-      <c r="A622" s="10"/>
+      <c r="A622" s="16"/>
     </row>
     <row r="623" ht="15.75" customHeight="1">
-      <c r="A623" s="10"/>
+      <c r="A623" s="16"/>
     </row>
     <row r="624" ht="15.75" customHeight="1">
-      <c r="A624" s="10"/>
+      <c r="A624" s="16"/>
     </row>
     <row r="625" ht="15.75" customHeight="1">
-      <c r="A625" s="10"/>
+      <c r="A625" s="16"/>
     </row>
     <row r="626" ht="15.75" customHeight="1">
-      <c r="A626" s="10"/>
+      <c r="A626" s="16"/>
     </row>
     <row r="627" ht="15.75" customHeight="1">
-      <c r="A627" s="10"/>
+      <c r="A627" s="16"/>
     </row>
     <row r="628" ht="15.75" customHeight="1">
-      <c r="A628" s="10"/>
+      <c r="A628" s="16"/>
     </row>
     <row r="629" ht="15.75" customHeight="1">
-      <c r="A629" s="10"/>
+      <c r="A629" s="16"/>
     </row>
     <row r="630" ht="15.75" customHeight="1">
-      <c r="A630" s="10"/>
+      <c r="A630" s="16"/>
     </row>
     <row r="631" ht="15.75" customHeight="1">
-      <c r="A631" s="10"/>
+      <c r="A631" s="16"/>
     </row>
     <row r="632" ht="15.75" customHeight="1">
-      <c r="A632" s="10"/>
+      <c r="A632" s="16"/>
     </row>
     <row r="633" ht="15.75" customHeight="1">
-      <c r="A633" s="10"/>
+      <c r="A633" s="16"/>
     </row>
     <row r="634" ht="15.75" customHeight="1">
-      <c r="A634" s="10"/>
+      <c r="A634" s="16"/>
     </row>
     <row r="635" ht="15.75" customHeight="1">
-      <c r="A635" s="10"/>
+      <c r="A635" s="16"/>
     </row>
     <row r="636" ht="15.75" customHeight="1">
-      <c r="A636" s="10"/>
+      <c r="A636" s="16"/>
     </row>
     <row r="637" ht="15.75" customHeight="1">
-      <c r="A637" s="10"/>
+      <c r="A637" s="16"/>
     </row>
     <row r="638" ht="15.75" customHeight="1">
-      <c r="A638" s="10"/>
+      <c r="A638" s="16"/>
     </row>
     <row r="639" ht="15.75" customHeight="1">
-      <c r="A639" s="10"/>
+      <c r="A639" s="16"/>
     </row>
     <row r="640" ht="15.75" customHeight="1">
-      <c r="A640" s="10"/>
+      <c r="A640" s="16"/>
     </row>
     <row r="641" ht="15.75" customHeight="1">
-      <c r="A641" s="10"/>
+      <c r="A641" s="16"/>
     </row>
     <row r="642" ht="15.75" customHeight="1">
-      <c r="A642" s="10"/>
+      <c r="A642" s="16"/>
     </row>
     <row r="643" ht="15.75" customHeight="1">
-      <c r="A643" s="10"/>
+      <c r="A643" s="16"/>
     </row>
     <row r="644" ht="15.75" customHeight="1">
-      <c r="A644" s="10"/>
+      <c r="A644" s="16"/>
     </row>
     <row r="645" ht="15.75" customHeight="1">
-      <c r="A645" s="10"/>
+      <c r="A645" s="16"/>
     </row>
     <row r="646" ht="15.75" customHeight="1">
-      <c r="A646" s="10"/>
+      <c r="A646" s="16"/>
     </row>
     <row r="647" ht="15.75" customHeight="1">
-      <c r="A647" s="10"/>
+      <c r="A647" s="16"/>
     </row>
     <row r="648" ht="15.75" customHeight="1">
-      <c r="A648" s="10"/>
+      <c r="A648" s="16"/>
     </row>
     <row r="649" ht="15.75" customHeight="1">
-      <c r="A649" s="10"/>
+      <c r="A649" s="16"/>
     </row>
     <row r="650" ht="15.75" customHeight="1">
-      <c r="A650" s="10"/>
+      <c r="A650" s="16"/>
     </row>
     <row r="651" ht="15.75" customHeight="1">
-      <c r="A651" s="10"/>
+      <c r="A651" s="16"/>
     </row>
     <row r="652" ht="15.75" customHeight="1">
-      <c r="A652" s="10"/>
+      <c r="A652" s="16"/>
     </row>
     <row r="653" ht="15.75" customHeight="1">
-      <c r="A653" s="10"/>
+      <c r="A653" s="16"/>
     </row>
     <row r="654" ht="15.75" customHeight="1">
-      <c r="A654" s="10"/>
+      <c r="A654" s="16"/>
     </row>
     <row r="655" ht="15.75" customHeight="1">
-      <c r="A655" s="10"/>
+      <c r="A655" s="16"/>
     </row>
     <row r="656" ht="15.75" customHeight="1">
-      <c r="A656" s="10"/>
+      <c r="A656" s="16"/>
     </row>
     <row r="657" ht="15.75" customHeight="1">
-      <c r="A657" s="10"/>
+      <c r="A657" s="16"/>
     </row>
     <row r="658" ht="15.75" customHeight="1">
-      <c r="A658" s="10"/>
+      <c r="A658" s="16"/>
     </row>
     <row r="659" ht="15.75" customHeight="1">
-      <c r="A659" s="10"/>
+      <c r="A659" s="16"/>
     </row>
     <row r="660" ht="15.75" customHeight="1">
-      <c r="A660" s="10"/>
+      <c r="A660" s="16"/>
     </row>
     <row r="661" ht="15.75" customHeight="1">
-      <c r="A661" s="10"/>
+      <c r="A661" s="16"/>
     </row>
     <row r="662" ht="15.75" customHeight="1">
-      <c r="A662" s="10"/>
+      <c r="A662" s="16"/>
     </row>
     <row r="663" ht="15.75" customHeight="1">
-      <c r="A663" s="10"/>
+      <c r="A663" s="16"/>
     </row>
     <row r="664" ht="15.75" customHeight="1">
-      <c r="A664" s="10"/>
+      <c r="A664" s="16"/>
     </row>
     <row r="665" ht="15.75" customHeight="1">
-      <c r="A665" s="10"/>
+      <c r="A665" s="16"/>
     </row>
     <row r="666" ht="15.75" customHeight="1">
-      <c r="A666" s="10"/>
+      <c r="A666" s="16"/>
     </row>
     <row r="667" ht="15.75" customHeight="1">
-      <c r="A667" s="10"/>
+      <c r="A667" s="16"/>
     </row>
     <row r="668" ht="15.75" customHeight="1">
-      <c r="A668" s="10"/>
+      <c r="A668" s="16"/>
     </row>
     <row r="669" ht="15.75" customHeight="1">
-      <c r="A669" s="10"/>
+      <c r="A669" s="16"/>
     </row>
     <row r="670" ht="15.75" customHeight="1">
-      <c r="A670" s="10"/>
+      <c r="A670" s="16"/>
     </row>
     <row r="671" ht="15.75" customHeight="1">
-      <c r="A671" s="10"/>
+      <c r="A671" s="16"/>
     </row>
     <row r="672" ht="15.75" customHeight="1">
-      <c r="A672" s="10"/>
+      <c r="A672" s="16"/>
     </row>
     <row r="673" ht="15.75" customHeight="1">
-      <c r="A673" s="10"/>
+      <c r="A673" s="16"/>
     </row>
     <row r="674" ht="15.75" customHeight="1">
-      <c r="A674" s="10"/>
+      <c r="A674" s="16"/>
     </row>
     <row r="675" ht="15.75" customHeight="1">
-      <c r="A675" s="10"/>
+      <c r="A675" s="16"/>
     </row>
     <row r="676" ht="15.75" customHeight="1">
-      <c r="A676" s="10"/>
+      <c r="A676" s="16"/>
     </row>
     <row r="677" ht="15.75" customHeight="1">
-      <c r="A677" s="10"/>
+      <c r="A677" s="16"/>
     </row>
     <row r="678" ht="15.75" customHeight="1">
-      <c r="A678" s="10"/>
+      <c r="A678" s="16"/>
     </row>
     <row r="679" ht="15.75" customHeight="1">
-      <c r="A679" s="10"/>
+      <c r="A679" s="16"/>
     </row>
     <row r="680" ht="15.75" customHeight="1">
-      <c r="A680" s="10"/>
+      <c r="A680" s="16"/>
     </row>
     <row r="681" ht="15.75" customHeight="1">
-      <c r="A681" s="10"/>
+      <c r="A681" s="16"/>
     </row>
     <row r="682" ht="15.75" customHeight="1">
-      <c r="A682" s="10"/>
+      <c r="A682" s="16"/>
     </row>
     <row r="683" ht="15.75" customHeight="1">
-      <c r="A683" s="10"/>
+      <c r="A683" s="16"/>
     </row>
     <row r="684" ht="15.75" customHeight="1">
-      <c r="A684" s="10"/>
+      <c r="A684" s="16"/>
     </row>
     <row r="685" ht="15.75" customHeight="1">
-      <c r="A685" s="10"/>
+      <c r="A685" s="16"/>
     </row>
     <row r="686" ht="15.75" customHeight="1">
-      <c r="A686" s="10"/>
+      <c r="A686" s="16"/>
     </row>
     <row r="687" ht="15.75" customHeight="1">
-      <c r="A687" s="10"/>
+      <c r="A687" s="16"/>
     </row>
     <row r="688" ht="15.75" customHeight="1">
-      <c r="A688" s="10"/>
+      <c r="A688" s="16"/>
     </row>
     <row r="689" ht="15.75" customHeight="1">
-      <c r="A689" s="10"/>
+      <c r="A689" s="16"/>
     </row>
     <row r="690" ht="15.75" customHeight="1">
-      <c r="A690" s="10"/>
+      <c r="A690" s="16"/>
     </row>
     <row r="691" ht="15.75" customHeight="1">
-      <c r="A691" s="10"/>
+      <c r="A691" s="16"/>
     </row>
     <row r="692" ht="15.75" customHeight="1">
-      <c r="A692" s="10"/>
+      <c r="A692" s="16"/>
     </row>
     <row r="693" ht="15.75" customHeight="1">
-      <c r="A693" s="10"/>
+      <c r="A693" s="16"/>
     </row>
     <row r="694" ht="15.75" customHeight="1">
-      <c r="A694" s="10"/>
+      <c r="A694" s="16"/>
     </row>
     <row r="695" ht="15.75" customHeight="1">
-      <c r="A695" s="10"/>
+      <c r="A695" s="16"/>
     </row>
     <row r="696" ht="15.75" customHeight="1">
-      <c r="A696" s="10"/>
+      <c r="A696" s="16"/>
     </row>
     <row r="697" ht="15.75" customHeight="1">
-      <c r="A697" s="10"/>
+      <c r="A697" s="16"/>
     </row>
     <row r="698" ht="15.75" customHeight="1">
-      <c r="A698" s="10"/>
+      <c r="A698" s="16"/>
     </row>
     <row r="699" ht="15.75" customHeight="1">
-      <c r="A699" s="10"/>
+      <c r="A699" s="16"/>
     </row>
     <row r="700" ht="15.75" customHeight="1">
-      <c r="A700" s="10"/>
+      <c r="A700" s="16"/>
     </row>
     <row r="701" ht="15.75" customHeight="1">
-      <c r="A701" s="10"/>
+      <c r="A701" s="16"/>
     </row>
     <row r="702" ht="15.75" customHeight="1">
-      <c r="A702" s="10"/>
+      <c r="A702" s="16"/>
     </row>
     <row r="703" ht="15.75" customHeight="1">
-      <c r="A703" s="10"/>
+      <c r="A703" s="16"/>
     </row>
     <row r="704" ht="15.75" customHeight="1">
-      <c r="A704" s="10"/>
+      <c r="A704" s="16"/>
     </row>
     <row r="705" ht="15.75" customHeight="1">
-      <c r="A705" s="10"/>
+      <c r="A705" s="16"/>
     </row>
     <row r="706" ht="15.75" customHeight="1">
-      <c r="A706" s="10"/>
+      <c r="A706" s="16"/>
     </row>
     <row r="707" ht="15.75" customHeight="1">
-      <c r="A707" s="10"/>
+      <c r="A707" s="16"/>
     </row>
     <row r="708" ht="15.75" customHeight="1">
-      <c r="A708" s="10"/>
+      <c r="A708" s="16"/>
     </row>
     <row r="709" ht="15.75" customHeight="1">
-      <c r="A709" s="10"/>
+      <c r="A709" s="16"/>
     </row>
     <row r="710" ht="15.75" customHeight="1">
-      <c r="A710" s="10"/>
+      <c r="A710" s="16"/>
     </row>
     <row r="711" ht="15.75" customHeight="1">
-      <c r="A711" s="10"/>
+      <c r="A711" s="16"/>
     </row>
     <row r="712" ht="15.75" customHeight="1">
-      <c r="A712" s="10"/>
+      <c r="A712" s="16"/>
     </row>
     <row r="713" ht="15.75" customHeight="1">
-      <c r="A713" s="10"/>
+      <c r="A713" s="16"/>
     </row>
     <row r="714" ht="15.75" customHeight="1">
-      <c r="A714" s="10"/>
+      <c r="A714" s="16"/>
     </row>
     <row r="715" ht="15.75" customHeight="1">
-      <c r="A715" s="10"/>
+      <c r="A715" s="16"/>
     </row>
     <row r="716" ht="15.75" customHeight="1">
-      <c r="A716" s="10"/>
+      <c r="A716" s="16"/>
     </row>
     <row r="717" ht="15.75" customHeight="1">
-      <c r="A717" s="10"/>
+      <c r="A717" s="16"/>
     </row>
     <row r="718" ht="15.75" customHeight="1">
-      <c r="A718" s="10"/>
+      <c r="A718" s="16"/>
     </row>
     <row r="719" ht="15.75" customHeight="1">
-      <c r="A719" s="10"/>
+      <c r="A719" s="16"/>
     </row>
     <row r="720" ht="15.75" customHeight="1">
-      <c r="A720" s="10"/>
+      <c r="A720" s="16"/>
     </row>
     <row r="721" ht="15.75" customHeight="1">
-      <c r="A721" s="10"/>
+      <c r="A721" s="16"/>
     </row>
     <row r="722" ht="15.75" customHeight="1">
-      <c r="A722" s="10"/>
+      <c r="A722" s="16"/>
     </row>
     <row r="723" ht="15.75" customHeight="1">
-      <c r="A723" s="10"/>
+      <c r="A723" s="16"/>
     </row>
     <row r="724" ht="15.75" customHeight="1">
-      <c r="A724" s="10"/>
+      <c r="A724" s="16"/>
     </row>
     <row r="725" ht="15.75" customHeight="1">
-      <c r="A725" s="10"/>
+      <c r="A725" s="16"/>
     </row>
     <row r="726" ht="15.75" customHeight="1">
-      <c r="A726" s="10"/>
+      <c r="A726" s="16"/>
     </row>
     <row r="727" ht="15.75" customHeight="1">
-      <c r="A727" s="10"/>
+      <c r="A727" s="16"/>
     </row>
     <row r="728" ht="15.75" customHeight="1">
-      <c r="A728" s="10"/>
+      <c r="A728" s="16"/>
     </row>
     <row r="729" ht="15.75" customHeight="1">
-      <c r="A729" s="10"/>
+      <c r="A729" s="16"/>
     </row>
     <row r="730" ht="15.75" customHeight="1">
-      <c r="A730" s="10"/>
+      <c r="A730" s="16"/>
     </row>
     <row r="731" ht="15.75" customHeight="1">
-      <c r="A731" s="10"/>
+      <c r="A731" s="16"/>
     </row>
     <row r="732" ht="15.75" customHeight="1">
-      <c r="A732" s="10"/>
+      <c r="A732" s="16"/>
     </row>
     <row r="733" ht="15.75" customHeight="1">
-      <c r="A733" s="10"/>
+      <c r="A733" s="16"/>
     </row>
     <row r="734" ht="15.75" customHeight="1">
-      <c r="A734" s="10"/>
+      <c r="A734" s="16"/>
     </row>
     <row r="735" ht="15.75" customHeight="1">
-      <c r="A735" s="10"/>
+      <c r="A735" s="16"/>
     </row>
     <row r="736" ht="15.75" customHeight="1">
-      <c r="A736" s="10"/>
+      <c r="A736" s="16"/>
     </row>
     <row r="737" ht="15.75" customHeight="1">
-      <c r="A737" s="10"/>
+      <c r="A737" s="16"/>
     </row>
     <row r="738" ht="15.75" customHeight="1">
-      <c r="A738" s="10"/>
+      <c r="A738" s="16"/>
     </row>
     <row r="739" ht="15.75" customHeight="1">
-      <c r="A739" s="10"/>
+      <c r="A739" s="16"/>
     </row>
     <row r="740" ht="15.75" customHeight="1">
-      <c r="A740" s="10"/>
+      <c r="A740" s="16"/>
     </row>
     <row r="741" ht="15.75" customHeight="1">
-      <c r="A741" s="10"/>
+      <c r="A741" s="16"/>
     </row>
     <row r="742" ht="15.75" customHeight="1">
-      <c r="A742" s="10"/>
+      <c r="A742" s="16"/>
     </row>
     <row r="743" ht="15.75" customHeight="1">
-      <c r="A743" s="10"/>
+      <c r="A743" s="16"/>
     </row>
     <row r="744" ht="15.75" customHeight="1">
-      <c r="A744" s="10"/>
+      <c r="A744" s="16"/>
     </row>
     <row r="745" ht="15.75" customHeight="1">
-      <c r="A745" s="10"/>
+      <c r="A745" s="16"/>
     </row>
     <row r="746" ht="15.75" customHeight="1">
-      <c r="A746" s="10"/>
+      <c r="A746" s="16"/>
     </row>
     <row r="747" ht="15.75" customHeight="1">
-      <c r="A747" s="10"/>
+      <c r="A747" s="16"/>
     </row>
     <row r="748" ht="15.75" customHeight="1">
-      <c r="A748" s="10"/>
+      <c r="A748" s="16"/>
     </row>
     <row r="749" ht="15.75" customHeight="1">
-      <c r="A749" s="10"/>
+      <c r="A749" s="16"/>
     </row>
     <row r="750" ht="15.75" customHeight="1">
-      <c r="A750" s="10"/>
+      <c r="A750" s="16"/>
     </row>
     <row r="751" ht="15.75" customHeight="1">
-      <c r="A751" s="10"/>
+      <c r="A751" s="16"/>
     </row>
     <row r="752" ht="15.75" customHeight="1">
-      <c r="A752" s="10"/>
+      <c r="A752" s="16"/>
     </row>
     <row r="753" ht="15.75" customHeight="1">
-      <c r="A753" s="10"/>
+      <c r="A753" s="16"/>
     </row>
     <row r="754" ht="15.75" customHeight="1">
-      <c r="A754" s="10"/>
+      <c r="A754" s="16"/>
     </row>
     <row r="755" ht="15.75" customHeight="1">
-      <c r="A755" s="10"/>
+      <c r="A755" s="16"/>
     </row>
     <row r="756" ht="15.75" customHeight="1">
-      <c r="A756" s="10"/>
+      <c r="A756" s="16"/>
     </row>
     <row r="757" ht="15.75" customHeight="1">
-      <c r="A757" s="10"/>
+      <c r="A757" s="16"/>
     </row>
     <row r="758" ht="15.75" customHeight="1">
-      <c r="A758" s="10"/>
+      <c r="A758" s="16"/>
     </row>
     <row r="759" ht="15.75" customHeight="1">
-      <c r="A759" s="10"/>
+      <c r="A759" s="16"/>
     </row>
     <row r="760" ht="15.75" customHeight="1">
-      <c r="A760" s="10"/>
+      <c r="A760" s="16"/>
     </row>
     <row r="761" ht="15.75" customHeight="1">
-      <c r="A761" s="10"/>
+      <c r="A761" s="16"/>
     </row>
     <row r="762" ht="15.75" customHeight="1">
-      <c r="A762" s="10"/>
+      <c r="A762" s="16"/>
     </row>
     <row r="763" ht="15.75" customHeight="1">
-      <c r="A763" s="10"/>
+      <c r="A763" s="16"/>
     </row>
     <row r="764" ht="15.75" customHeight="1">
-      <c r="A764" s="10"/>
+      <c r="A764" s="16"/>
     </row>
     <row r="765" ht="15.75" customHeight="1">
-      <c r="A765" s="10"/>
+      <c r="A765" s="16"/>
     </row>
     <row r="766" ht="15.75" customHeight="1">
-      <c r="A766" s="10"/>
+      <c r="A766" s="16"/>
     </row>
     <row r="767" ht="15.75" customHeight="1">
-      <c r="A767" s="10"/>
+      <c r="A767" s="16"/>
     </row>
     <row r="768" ht="15.75" customHeight="1">
-      <c r="A768" s="10"/>
+      <c r="A768" s="16"/>
     </row>
     <row r="769" ht="15.75" customHeight="1">
-      <c r="A769" s="10"/>
+      <c r="A769" s="16"/>
     </row>
     <row r="770" ht="15.75" customHeight="1">
-      <c r="A770" s="10"/>
+      <c r="A770" s="16"/>
     </row>
     <row r="771" ht="15.75" customHeight="1">
-      <c r="A771" s="10"/>
+      <c r="A771" s="16"/>
     </row>
     <row r="772" ht="15.75" customHeight="1">
-      <c r="A772" s="10"/>
+      <c r="A772" s="16"/>
     </row>
     <row r="773" ht="15.75" customHeight="1">
-      <c r="A773" s="10"/>
+      <c r="A773" s="16"/>
     </row>
     <row r="774" ht="15.75" customHeight="1">
-      <c r="A774" s="10"/>
+      <c r="A774" s="16"/>
     </row>
     <row r="775" ht="15.75" customHeight="1">
-      <c r="A775" s="10"/>
+      <c r="A775" s="16"/>
     </row>
     <row r="776" ht="15.75" customHeight="1">
-      <c r="A776" s="10"/>
+      <c r="A776" s="16"/>
     </row>
     <row r="777" ht="15.75" customHeight="1">
-      <c r="A777" s="10"/>
+      <c r="A777" s="16"/>
     </row>
     <row r="778" ht="15.75" customHeight="1">
-      <c r="A778" s="10"/>
+      <c r="A778" s="16"/>
     </row>
     <row r="779" ht="15.75" customHeight="1">
-      <c r="A779" s="10"/>
+      <c r="A779" s="16"/>
     </row>
     <row r="780" ht="15.75" customHeight="1">
-      <c r="A780" s="10"/>
+      <c r="A780" s="16"/>
     </row>
     <row r="781" ht="15.75" customHeight="1">
-      <c r="A781" s="10"/>
+      <c r="A781" s="16"/>
     </row>
     <row r="782" ht="15.75" customHeight="1">
-      <c r="A782" s="10"/>
+      <c r="A782" s="16"/>
     </row>
     <row r="783" ht="15.75" customHeight="1">
-      <c r="A783" s="10"/>
+      <c r="A783" s="16"/>
     </row>
     <row r="784" ht="15.75" customHeight="1">
-      <c r="A784" s="10"/>
+      <c r="A784" s="16"/>
     </row>
     <row r="785" ht="15.75" customHeight="1">
-      <c r="A785" s="10"/>
+      <c r="A785" s="16"/>
     </row>
     <row r="786" ht="15.75" customHeight="1">
-      <c r="A786" s="10"/>
+      <c r="A786" s="16"/>
     </row>
     <row r="787" ht="15.75" customHeight="1">
-      <c r="A787" s="10"/>
+      <c r="A787" s="16"/>
     </row>
     <row r="788" ht="15.75" customHeight="1">
-      <c r="A788" s="10"/>
+      <c r="A788" s="16"/>
     </row>
     <row r="789" ht="15.75" customHeight="1">
-      <c r="A789" s="10"/>
+      <c r="A789" s="16"/>
     </row>
     <row r="790" ht="15.75" customHeight="1">
-      <c r="A790" s="10"/>
+      <c r="A790" s="16"/>
     </row>
     <row r="791" ht="15.75" customHeight="1">
-      <c r="A791" s="10"/>
+      <c r="A791" s="16"/>
     </row>
     <row r="792" ht="15.75" customHeight="1">
-      <c r="A792" s="10"/>
+      <c r="A792" s="16"/>
     </row>
     <row r="793" ht="15.75" customHeight="1">
-      <c r="A793" s="10"/>
+      <c r="A793" s="16"/>
     </row>
     <row r="794" ht="15.75" customHeight="1">
-      <c r="A794" s="10"/>
+      <c r="A794" s="16"/>
     </row>
     <row r="795" ht="15.75" customHeight="1">
-      <c r="A795" s="10"/>
+      <c r="A795" s="16"/>
     </row>
     <row r="796" ht="15.75" customHeight="1">
-      <c r="A796" s="10"/>
+      <c r="A796" s="16"/>
     </row>
     <row r="797" ht="15.75" customHeight="1">
-      <c r="A797" s="10"/>
+      <c r="A797" s="16"/>
     </row>
     <row r="798" ht="15.75" customHeight="1">
-      <c r="A798" s="10"/>
+      <c r="A798" s="16"/>
     </row>
     <row r="799" ht="15.75" customHeight="1">
-      <c r="A799" s="10"/>
+      <c r="A799" s="16"/>
     </row>
     <row r="800" ht="15.75" customHeight="1">
-      <c r="A800" s="10"/>
+      <c r="A800" s="16"/>
     </row>
     <row r="801" ht="15.75" customHeight="1">
-      <c r="A801" s="10"/>
+      <c r="A801" s="16"/>
     </row>
     <row r="802" ht="15.75" customHeight="1">
-      <c r="A802" s="10"/>
+      <c r="A802" s="16"/>
     </row>
     <row r="803" ht="15.75" customHeight="1">
-      <c r="A803" s="10"/>
+      <c r="A803" s="16"/>
     </row>
     <row r="804" ht="15.75" customHeight="1">
-      <c r="A804" s="10"/>
+      <c r="A804" s="16"/>
     </row>
     <row r="805" ht="15.75" customHeight="1">
-      <c r="A805" s="10"/>
+      <c r="A805" s="16"/>
     </row>
     <row r="806" ht="15.75" customHeight="1">
-      <c r="A806" s="10"/>
+      <c r="A806" s="16"/>
     </row>
     <row r="807" ht="15.75" customHeight="1">
-      <c r="A807" s="10"/>
+      <c r="A807" s="16"/>
     </row>
     <row r="808" ht="15.75" customHeight="1">
-      <c r="A808" s="10"/>
+      <c r="A808" s="16"/>
     </row>
     <row r="809" ht="15.75" customHeight="1">
-      <c r="A809" s="10"/>
+      <c r="A809" s="16"/>
     </row>
     <row r="810" ht="15.75" customHeight="1">
-      <c r="A810" s="10"/>
+      <c r="A810" s="16"/>
     </row>
     <row r="811" ht="15.75" customHeight="1">
-      <c r="A811" s="10"/>
+      <c r="A811" s="16"/>
     </row>
     <row r="812" ht="15.75" customHeight="1">
-      <c r="A812" s="10"/>
+      <c r="A812" s="16"/>
     </row>
     <row r="813" ht="15.75" customHeight="1">
-      <c r="A813" s="10"/>
+      <c r="A813" s="16"/>
     </row>
     <row r="814" ht="15.75" customHeight="1">
-      <c r="A814" s="10"/>
+      <c r="A814" s="16"/>
     </row>
     <row r="815" ht="15.75" customHeight="1">
-      <c r="A815" s="10"/>
+      <c r="A815" s="16"/>
     </row>
     <row r="816" ht="15.75" customHeight="1">
-      <c r="A816" s="10"/>
+      <c r="A816" s="16"/>
     </row>
     <row r="817" ht="15.75" customHeight="1">
-      <c r="A817" s="10"/>
+      <c r="A817" s="16"/>
     </row>
     <row r="818" ht="15.75" customHeight="1">
-      <c r="A818" s="10"/>
+      <c r="A818" s="16"/>
     </row>
     <row r="819" ht="15.75" customHeight="1">
-      <c r="A819" s="10"/>
+      <c r="A819" s="16"/>
     </row>
     <row r="820" ht="15.75" customHeight="1">
-      <c r="A820" s="10"/>
+      <c r="A820" s="16"/>
     </row>
     <row r="821" ht="15.75" customHeight="1">
-      <c r="A821" s="10"/>
+      <c r="A821" s="16"/>
     </row>
     <row r="822" ht="15.75" customHeight="1">
-      <c r="A822" s="10"/>
+      <c r="A822" s="16"/>
     </row>
     <row r="823" ht="15.75" customHeight="1">
-      <c r="A823" s="10"/>
+      <c r="A823" s="16"/>
     </row>
     <row r="824" ht="15.75" customHeight="1">
-      <c r="A824" s="10"/>
+      <c r="A824" s="16"/>
     </row>
     <row r="825" ht="15.75" customHeight="1">
-      <c r="A825" s="10"/>
+      <c r="A825" s="16"/>
     </row>
     <row r="826" ht="15.75" customHeight="1">
-      <c r="A826" s="10"/>
+      <c r="A826" s="16"/>
     </row>
     <row r="827" ht="15.75" customHeight="1">
-      <c r="A827" s="10"/>
+      <c r="A827" s="16"/>
     </row>
     <row r="828" ht="15.75" customHeight="1">
-      <c r="A828" s="10"/>
+      <c r="A828" s="16"/>
     </row>
     <row r="829" ht="15.75" customHeight="1">
-      <c r="A829" s="10"/>
+      <c r="A829" s="16"/>
     </row>
     <row r="830" ht="15.75" customHeight="1">
-      <c r="A830" s="10"/>
+      <c r="A830" s="16"/>
     </row>
     <row r="831" ht="15.75" customHeight="1">
-      <c r="A831" s="10"/>
+      <c r="A831" s="16"/>
     </row>
     <row r="832" ht="15.75" customHeight="1">
-      <c r="A832" s="10"/>
+      <c r="A832" s="16"/>
     </row>
     <row r="833" ht="15.75" customHeight="1">
-      <c r="A833" s="10"/>
+      <c r="A833" s="16"/>
     </row>
     <row r="834" ht="15.75" customHeight="1">
-      <c r="A834" s="10"/>
+      <c r="A834" s="16"/>
     </row>
     <row r="835" ht="15.75" customHeight="1">
-      <c r="A835" s="10"/>
+      <c r="A835" s="16"/>
     </row>
     <row r="836" ht="15.75" customHeight="1">
-      <c r="A836" s="10"/>
+      <c r="A836" s="16"/>
     </row>
     <row r="837" ht="15.75" customHeight="1">
-      <c r="A837" s="10"/>
+      <c r="A837" s="16"/>
     </row>
     <row r="838" ht="15.75" customHeight="1">
-      <c r="A838" s="10"/>
+      <c r="A838" s="16"/>
     </row>
     <row r="839" ht="15.75" customHeight="1">
-      <c r="A839" s="10"/>
+      <c r="A839" s="16"/>
     </row>
     <row r="840" ht="15.75" customHeight="1">
-      <c r="A840" s="10"/>
+      <c r="A840" s="16"/>
     </row>
     <row r="841" ht="15.75" customHeight="1">
-      <c r="A841" s="10"/>
+      <c r="A841" s="16"/>
     </row>
     <row r="842" ht="15.75" customHeight="1">
-      <c r="A842" s="10"/>
+      <c r="A842" s="16"/>
     </row>
     <row r="843" ht="15.75" customHeight="1">
-      <c r="A843" s="10"/>
+      <c r="A843" s="16"/>
     </row>
     <row r="844" ht="15.75" customHeight="1">
-      <c r="A844" s="10"/>
+      <c r="A844" s="16"/>
     </row>
     <row r="845" ht="15.75" customHeight="1">
-      <c r="A845" s="10"/>
+      <c r="A845" s="16"/>
     </row>
     <row r="846" ht="15.75" customHeight="1">
-      <c r="A846" s="10"/>
+      <c r="A846" s="16"/>
     </row>
     <row r="847" ht="15.75" customHeight="1">
-      <c r="A847" s="10"/>
+      <c r="A847" s="16"/>
     </row>
     <row r="848" ht="15.75" customHeight="1">
-      <c r="A848" s="10"/>
+      <c r="A848" s="16"/>
     </row>
     <row r="849" ht="15.75" customHeight="1">
-      <c r="A849" s="10"/>
+      <c r="A849" s="16"/>
     </row>
     <row r="850" ht="15.75" customHeight="1">
-      <c r="A850" s="10"/>
+      <c r="A850" s="16"/>
     </row>
     <row r="851" ht="15.75" customHeight="1">
-      <c r="A851" s="10"/>
+      <c r="A851" s="16"/>
     </row>
     <row r="852" ht="15.75" customHeight="1">
-      <c r="A852" s="10"/>
+      <c r="A852" s="16"/>
     </row>
     <row r="853" ht="15.75" customHeight="1">
-      <c r="A853" s="10"/>
+      <c r="A853" s="16"/>
     </row>
     <row r="854" ht="15.75" customHeight="1">
-      <c r="A854" s="10"/>
+      <c r="A854" s="16"/>
     </row>
     <row r="855" ht="15.75" customHeight="1">
-      <c r="A855" s="10"/>
+      <c r="A855" s="16"/>
     </row>
     <row r="856" ht="15.75" customHeight="1">
-      <c r="A856" s="10"/>
+      <c r="A856" s="16"/>
     </row>
     <row r="857" ht="15.75" customHeight="1">
-      <c r="A857" s="10"/>
+      <c r="A857" s="16"/>
     </row>
     <row r="858" ht="15.75" customHeight="1">
-      <c r="A858" s="10"/>
+      <c r="A858" s="16"/>
     </row>
     <row r="859" ht="15.75" customHeight="1">
-      <c r="A859" s="10"/>
+      <c r="A859" s="16"/>
     </row>
     <row r="860" ht="15.75" customHeight="1">
-      <c r="A860" s="10"/>
+      <c r="A860" s="16"/>
     </row>
     <row r="861" ht="15.75" customHeight="1">
-      <c r="A861" s="10"/>
+      <c r="A861" s="16"/>
     </row>
     <row r="862" ht="15.75" customHeight="1">
-      <c r="A862" s="10"/>
+      <c r="A862" s="16"/>
     </row>
     <row r="863" ht="15.75" customHeight="1">
-      <c r="A863" s="10"/>
+      <c r="A863" s="16"/>
     </row>
     <row r="864" ht="15.75" customHeight="1">
-      <c r="A864" s="10"/>
+      <c r="A864" s="16"/>
     </row>
     <row r="865" ht="15.75" customHeight="1">
-      <c r="A865" s="10"/>
+      <c r="A865" s="16"/>
     </row>
     <row r="866" ht="15.75" customHeight="1">
-      <c r="A866" s="10"/>
+      <c r="A866" s="16"/>
     </row>
     <row r="867" ht="15.75" customHeight="1">
-      <c r="A867" s="10"/>
+      <c r="A867" s="16"/>
     </row>
     <row r="868" ht="15.75" customHeight="1">
-      <c r="A868" s="10"/>
+      <c r="A868" s="16"/>
     </row>
     <row r="869" ht="15.75" customHeight="1">
-      <c r="A869" s="10"/>
+      <c r="A869" s="16"/>
     </row>
     <row r="870" ht="15.75" customHeight="1">
-      <c r="A870" s="10"/>
+      <c r="A870" s="16"/>
     </row>
     <row r="871" ht="15.75" customHeight="1">
-      <c r="A871" s="10"/>
+      <c r="A871" s="16"/>
     </row>
     <row r="872" ht="15.75" customHeight="1">
-      <c r="A872" s="10"/>
+      <c r="A872" s="16"/>
     </row>
     <row r="873" ht="15.75" customHeight="1">
-      <c r="A873" s="10"/>
+      <c r="A873" s="16"/>
     </row>
     <row r="874" ht="15.75" customHeight="1">
-      <c r="A874" s="10"/>
+      <c r="A874" s="16"/>
     </row>
     <row r="875" ht="15.75" customHeight="1">
-      <c r="A875" s="10"/>
+      <c r="A875" s="16"/>
     </row>
     <row r="876" ht="15.75" customHeight="1">
-      <c r="A876" s="10"/>
+      <c r="A876" s="16"/>
     </row>
     <row r="877" ht="15.75" customHeight="1">
-      <c r="A877" s="10"/>
+      <c r="A877" s="16"/>
     </row>
     <row r="878" ht="15.75" customHeight="1">
-      <c r="A878" s="10"/>
+      <c r="A878" s="16"/>
     </row>
     <row r="879" ht="15.75" customHeight="1">
-      <c r="A879" s="10"/>
+      <c r="A879" s="16"/>
     </row>
     <row r="880" ht="15.75" customHeight="1">
-      <c r="A880" s="10"/>
+      <c r="A880" s="16"/>
     </row>
     <row r="881" ht="15.75" customHeight="1">
-      <c r="A881" s="10"/>
+      <c r="A881" s="16"/>
     </row>
     <row r="882" ht="15.75" customHeight="1">
-      <c r="A882" s="10"/>
+      <c r="A882" s="16"/>
     </row>
     <row r="883" ht="15.75" customHeight="1">
-      <c r="A883" s="10"/>
+      <c r="A883" s="16"/>
     </row>
     <row r="884" ht="15.75" customHeight="1">
-      <c r="A884" s="10"/>
+      <c r="A884" s="16"/>
     </row>
     <row r="885" ht="15.75" customHeight="1">
-      <c r="A885" s="10"/>
+      <c r="A885" s="16"/>
     </row>
     <row r="886" ht="15.75" customHeight="1">
-      <c r="A886" s="10"/>
+      <c r="A886" s="16"/>
     </row>
     <row r="887" ht="15.75" customHeight="1">
-      <c r="A887" s="10"/>
+      <c r="A887" s="16"/>
     </row>
     <row r="888" ht="15.75" customHeight="1">
-      <c r="A888" s="10"/>
+      <c r="A888" s="16"/>
     </row>
     <row r="889" ht="15.75" customHeight="1">
-      <c r="A889" s="10"/>
+      <c r="A889" s="16"/>
     </row>
     <row r="890" ht="15.75" customHeight="1">
-      <c r="A890" s="10"/>
+      <c r="A890" s="16"/>
     </row>
     <row r="891" ht="15.75" customHeight="1">
-      <c r="A891" s="10"/>
+      <c r="A891" s="16"/>
     </row>
     <row r="892" ht="15.75" customHeight="1">
-      <c r="A892" s="10"/>
+      <c r="A892" s="16"/>
     </row>
     <row r="893" ht="15.75" customHeight="1">
-      <c r="A893" s="10"/>
+      <c r="A893" s="16"/>
     </row>
     <row r="894" ht="15.75" customHeight="1">
-      <c r="A894" s="10"/>
+      <c r="A894" s="16"/>
     </row>
     <row r="895" ht="15.75" customHeight="1">
-      <c r="A895" s="10"/>
+      <c r="A895" s="16"/>
     </row>
     <row r="896" ht="15.75" customHeight="1">
-      <c r="A896" s="10"/>
+      <c r="A896" s="16"/>
     </row>
     <row r="897" ht="15.75" customHeight="1">
-      <c r="A897" s="10"/>
+      <c r="A897" s="16"/>
     </row>
     <row r="898" ht="15.75" customHeight="1">
-      <c r="A898" s="10"/>
+      <c r="A898" s="16"/>
     </row>
     <row r="899" ht="15.75" customHeight="1">
-      <c r="A899" s="10"/>
+      <c r="A899" s="16"/>
     </row>
     <row r="900" ht="15.75" customHeight="1">
-      <c r="A900" s="10"/>
+      <c r="A900" s="16"/>
     </row>
     <row r="901" ht="15.75" customHeight="1">
-      <c r="A901" s="10"/>
+      <c r="A901" s="16"/>
     </row>
     <row r="902" ht="15.75" customHeight="1">
-      <c r="A902" s="10"/>
+      <c r="A902" s="16"/>
     </row>
     <row r="903" ht="15.75" customHeight="1">
-      <c r="A903" s="10"/>
+      <c r="A903" s="16"/>
     </row>
     <row r="904" ht="15.75" customHeight="1">
-      <c r="A904" s="10"/>
+      <c r="A904" s="16"/>
     </row>
     <row r="905" ht="15.75" customHeight="1">
-      <c r="A905" s="10"/>
+      <c r="A905" s="16"/>
     </row>
     <row r="906" ht="15.75" customHeight="1">
-      <c r="A906" s="10"/>
+      <c r="A906" s="16"/>
     </row>
     <row r="907" ht="15.75" customHeight="1">
-      <c r="A907" s="10"/>
+      <c r="A907" s="16"/>
     </row>
     <row r="908" ht="15.75" customHeight="1">
-      <c r="A908" s="10"/>
+      <c r="A908" s="16"/>
     </row>
     <row r="909" ht="15.75" customHeight="1">
-      <c r="A909" s="10"/>
+      <c r="A909" s="16"/>
     </row>
     <row r="910" ht="15.75" customHeight="1">
-      <c r="A910" s="10"/>
+      <c r="A910" s="16"/>
     </row>
     <row r="911" ht="15.75" customHeight="1">
-      <c r="A911" s="10"/>
+      <c r="A911" s="16"/>
     </row>
     <row r="912" ht="15.75" customHeight="1">
-      <c r="A912" s="10"/>
+      <c r="A912" s="16"/>
     </row>
     <row r="913" ht="15.75" customHeight="1">
-      <c r="A913" s="10"/>
+      <c r="A913" s="16"/>
     </row>
     <row r="914" ht="15.75" customHeight="1">
-      <c r="A914" s="10"/>
+      <c r="A914" s="16"/>
     </row>
     <row r="915" ht="15.75" customHeight="1">
-      <c r="A915" s="10"/>
+      <c r="A915" s="16"/>
     </row>
     <row r="916" ht="15.75" customHeight="1">
-      <c r="A916" s="10"/>
+      <c r="A916" s="16"/>
     </row>
     <row r="917" ht="15.75" customHeight="1">
-      <c r="A917" s="10"/>
+      <c r="A917" s="16"/>
     </row>
     <row r="918" ht="15.75" customHeight="1">
-      <c r="A918" s="10"/>
+      <c r="A918" s="16"/>
     </row>
     <row r="919" ht="15.75" customHeight="1">
-      <c r="A919" s="10"/>
+      <c r="A919" s="16"/>
     </row>
     <row r="920" ht="15.75" customHeight="1">
-      <c r="A920" s="10"/>
+      <c r="A920" s="16"/>
     </row>
     <row r="921" ht="15.75" customHeight="1">
-      <c r="A921" s="10"/>
+      <c r="A921" s="16"/>
     </row>
     <row r="922" ht="15.75" customHeight="1">
-      <c r="A922" s="10"/>
+      <c r="A922" s="16"/>
     </row>
     <row r="923" ht="15.75" customHeight="1">
-      <c r="A923" s="10"/>
+      <c r="A923" s="16"/>
     </row>
     <row r="924" ht="15.75" customHeight="1">
-      <c r="A924" s="10"/>
+      <c r="A924" s="16"/>
     </row>
     <row r="925" ht="15.75" customHeight="1">
-      <c r="A925" s="10"/>
+      <c r="A925" s="16"/>
     </row>
     <row r="926" ht="15.75" customHeight="1">
-      <c r="A926" s="10"/>
+      <c r="A926" s="16"/>
     </row>
     <row r="927" ht="15.75" customHeight="1">
-      <c r="A927" s="10"/>
+      <c r="A927" s="16"/>
     </row>
     <row r="928" ht="15.75" customHeight="1">
-      <c r="A928" s="10"/>
+      <c r="A928" s="16"/>
     </row>
     <row r="929" ht="15.75" customHeight="1">
-      <c r="A929" s="10"/>
+      <c r="A929" s="16"/>
     </row>
     <row r="930" ht="15.75" customHeight="1">
-      <c r="A930" s="10"/>
+      <c r="A930" s="16"/>
     </row>
     <row r="931" ht="15.75" customHeight="1">
-      <c r="A931" s="10"/>
+      <c r="A931" s="16"/>
     </row>
     <row r="932" ht="15.75" customHeight="1">
-      <c r="A932" s="10"/>
+      <c r="A932" s="16"/>
     </row>
     <row r="933" ht="15.75" customHeight="1">
-      <c r="A933" s="10"/>
+      <c r="A933" s="16"/>
     </row>
     <row r="934" ht="15.75" customHeight="1">
-      <c r="A934" s="10"/>
+      <c r="A934" s="16"/>
     </row>
     <row r="935" ht="15.75" customHeight="1">
-      <c r="A935" s="10"/>
+      <c r="A935" s="16"/>
     </row>
     <row r="936" ht="15.75" customHeight="1">
-      <c r="A936" s="10"/>
+      <c r="A936" s="16"/>
     </row>
     <row r="937" ht="15.75" customHeight="1">
-      <c r="A937" s="10"/>
+      <c r="A937" s="16"/>
     </row>
     <row r="938" ht="15.75" customHeight="1">
-      <c r="A938" s="10"/>
+      <c r="A938" s="16"/>
     </row>
     <row r="939" ht="15.75" customHeight="1">
-      <c r="A939" s="10"/>
+      <c r="A939" s="16"/>
     </row>
     <row r="940" ht="15.75" customHeight="1">
-      <c r="A940" s="10"/>
+      <c r="A940" s="16"/>
     </row>
     <row r="941" ht="15.75" customHeight="1">
-      <c r="A941" s="10"/>
+      <c r="A941" s="16"/>
     </row>
     <row r="942" ht="15.75" customHeight="1">
-      <c r="A942" s="10"/>
+      <c r="A942" s="16"/>
     </row>
     <row r="943" ht="15.75" customHeight="1">
-      <c r="A943" s="10"/>
+      <c r="A943" s="16"/>
     </row>
     <row r="944" ht="15.75" customHeight="1">
-      <c r="A944" s="10"/>
+      <c r="A944" s="16"/>
     </row>
     <row r="945" ht="15.75" customHeight="1">
-      <c r="A945" s="10"/>
+      <c r="A945" s="16"/>
     </row>
     <row r="946" ht="15.75" customHeight="1">
-      <c r="A946" s="10"/>
+      <c r="A946" s="16"/>
     </row>
     <row r="947" ht="15.75" customHeight="1">
-      <c r="A947" s="10"/>
+      <c r="A947" s="16"/>
     </row>
     <row r="948" ht="15.75" customHeight="1">
-      <c r="A948" s="10"/>
+      <c r="A948" s="16"/>
     </row>
     <row r="949" ht="15.75" customHeight="1">
-      <c r="A949" s="10"/>
+      <c r="A949" s="16"/>
     </row>
     <row r="950" ht="15.75" customHeight="1">
-      <c r="A950" s="10"/>
+      <c r="A950" s="16"/>
     </row>
     <row r="951" ht="15.75" customHeight="1">
-      <c r="A951" s="10"/>
+      <c r="A951" s="16"/>
     </row>
     <row r="952" ht="15.75" customHeight="1">
-      <c r="A952" s="10"/>
+      <c r="A952" s="16"/>
     </row>
     <row r="953" ht="15.75" customHeight="1">
-      <c r="A953" s="10"/>
+      <c r="A953" s="16"/>
     </row>
     <row r="954" ht="15.75" customHeight="1">
-      <c r="A954" s="10"/>
+      <c r="A954" s="16"/>
     </row>
     <row r="955" ht="15.75" customHeight="1">
-      <c r="A955" s="10"/>
+      <c r="A955" s="16"/>
     </row>
     <row r="956" ht="15.75" customHeight="1">
-      <c r="A956" s="10"/>
+      <c r="A956" s="16"/>
     </row>
     <row r="957" ht="15.75" customHeight="1">
-      <c r="A957" s="10"/>
+      <c r="A957" s="16"/>
     </row>
     <row r="958" ht="15.75" customHeight="1">
-      <c r="A958" s="10"/>
+      <c r="A958" s="16"/>
     </row>
     <row r="959" ht="15.75" customHeight="1">
-      <c r="A959" s="10"/>
+      <c r="A959" s="16"/>
     </row>
     <row r="960" ht="15.75" customHeight="1">
-      <c r="A960" s="10"/>
+      <c r="A960" s="16"/>
     </row>
     <row r="961" ht="15.75" customHeight="1">
-      <c r="A961" s="10"/>
+      <c r="A961" s="16"/>
     </row>
     <row r="962" ht="15.75" customHeight="1">
-      <c r="A962" s="10"/>
+      <c r="A962" s="16"/>
     </row>
     <row r="963" ht="15.75" customHeight="1">
-      <c r="A963" s="10"/>
+      <c r="A963" s="16"/>
     </row>
     <row r="964" ht="15.75" customHeight="1">
-      <c r="A964" s="10"/>
+      <c r="A964" s="16"/>
     </row>
     <row r="965" ht="15.75" customHeight="1">
-      <c r="A965" s="10"/>
+      <c r="A965" s="16"/>
     </row>
     <row r="966" ht="15.75" customHeight="1">
-      <c r="A966" s="10"/>
+      <c r="A966" s="16"/>
     </row>
     <row r="967" ht="15.75" customHeight="1">
-      <c r="A967" s="10"/>
+      <c r="A967" s="16"/>
     </row>
     <row r="968" ht="15.75" customHeight="1">
-      <c r="A968" s="10"/>
+      <c r="A968" s="16"/>
     </row>
     <row r="969" ht="15.75" customHeight="1">
-      <c r="A969" s="10"/>
+      <c r="A969" s="16"/>
     </row>
     <row r="970" ht="15.75" customHeight="1">
-      <c r="A970" s="10"/>
+      <c r="A970" s="16"/>
     </row>
     <row r="971" ht="15.75" customHeight="1">
-      <c r="A971" s="10"/>
+      <c r="A971" s="16"/>
     </row>
     <row r="972" ht="15.75" customHeight="1">
-      <c r="A972" s="10"/>
+      <c r="A972" s="16"/>
     </row>
     <row r="973" ht="15.75" customHeight="1">
-      <c r="A973" s="10"/>
+      <c r="A973" s="16"/>
     </row>
     <row r="974" ht="15.75" customHeight="1">
-      <c r="A974" s="10"/>
+      <c r="A974" s="16"/>
     </row>
     <row r="975" ht="15.75" customHeight="1">
-      <c r="A975" s="10"/>
+      <c r="A975" s="16"/>
     </row>
     <row r="976" ht="15.75" customHeight="1">
-      <c r="A976" s="10"/>
+      <c r="A976" s="16"/>
     </row>
     <row r="977" ht="15.75" customHeight="1">
-      <c r="A977" s="10"/>
+      <c r="A977" s="16"/>
     </row>
     <row r="978" ht="15.75" customHeight="1">
-      <c r="A978" s="10"/>
+      <c r="A978" s="16"/>
     </row>
     <row r="979" ht="15.75" customHeight="1">
-      <c r="A979" s="10"/>
+      <c r="A979" s="16"/>
     </row>
     <row r="980" ht="15.75" customHeight="1">
-      <c r="A980" s="10"/>
+      <c r="A980" s="16"/>
     </row>
     <row r="981" ht="15.75" customHeight="1">
-      <c r="A981" s="10"/>
+      <c r="A981" s="16"/>
     </row>
     <row r="982" ht="15.75" customHeight="1">
-      <c r="A982" s="10"/>
+      <c r="A982" s="16"/>
     </row>
     <row r="983" ht="15.75" customHeight="1">
-      <c r="A983" s="10"/>
+      <c r="A983" s="16"/>
     </row>
     <row r="984" ht="15.75" customHeight="1">
-      <c r="A984" s="10"/>
+      <c r="A984" s="16"/>
     </row>
     <row r="985" ht="15.75" customHeight="1">
-      <c r="A985" s="10"/>
+      <c r="A985" s="16"/>
     </row>
     <row r="986" ht="15.75" customHeight="1">
-      <c r="A986" s="10"/>
+      <c r="A986" s="16"/>
     </row>
     <row r="987" ht="15.75" customHeight="1">
-      <c r="A987" s="10"/>
+      <c r="A987" s="16"/>
     </row>
     <row r="988" ht="15.75" customHeight="1">
-      <c r="A988" s="10"/>
+      <c r="A988" s="16"/>
     </row>
     <row r="989" ht="15.75" customHeight="1">
-      <c r="A989" s="10"/>
+      <c r="A989" s="16"/>
     </row>
     <row r="990" ht="15.75" customHeight="1">
-      <c r="A990" s="10"/>
+      <c r="A990" s="16"/>
     </row>
     <row r="991" ht="15.75" customHeight="1">
-      <c r="A991" s="10"/>
+      <c r="A991" s="16"/>
     </row>
     <row r="992" ht="15.75" customHeight="1">
-      <c r="A992" s="10"/>
+      <c r="A992" s="16"/>
     </row>
     <row r="993" ht="15.75" customHeight="1">
-      <c r="A993" s="10"/>
+      <c r="A993" s="16"/>
     </row>
     <row r="994" ht="15.75" customHeight="1">
-      <c r="A994" s="10"/>
+      <c r="A994" s="16"/>
     </row>
     <row r="995" ht="15.75" customHeight="1">
-      <c r="A995" s="10"/>
+      <c r="A995" s="16"/>
     </row>
     <row r="996" ht="15.75" customHeight="1">
-      <c r="A996" s="10"/>
+      <c r="A996" s="16"/>
     </row>
     <row r="997" ht="15.75" customHeight="1">
-      <c r="A997" s="10"/>
+      <c r="A997" s="16"/>
     </row>
     <row r="998" ht="15.75" customHeight="1">
-      <c r="A998" s="10"/>
+      <c r="A998" s="16"/>
     </row>
     <row r="999" ht="15.75" customHeight="1">
-      <c r="A999" s="10"/>
+      <c r="A999" s="16"/>
     </row>
     <row r="1000" ht="15.75" customHeight="1">
-      <c r="A1000" s="10"/>
+      <c r="A1000" s="16"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -3901,18 +4005,20 @@
     <hyperlink r:id="rId3" ref="F4"/>
     <hyperlink r:id="rId4" ref="F5"/>
     <hyperlink r:id="rId5" ref="F6"/>
-    <hyperlink r:id="rId6" location=":~:text=Meta%20robots%20%3A%20d%C3%A9finition%20et%20code%20HTML&amp;text=La%20meta%20meta%20robots%20est,la%20page%20(robots%20noindex)." ref="F7"/>
+    <hyperlink r:id="rId6" ref="F7"/>
     <hyperlink r:id="rId7" ref="F8"/>
     <hyperlink r:id="rId8" ref="F9"/>
     <hyperlink r:id="rId9" ref="F10"/>
-    <hyperlink r:id="rId10" ref="F11"/>
+    <hyperlink r:id="rId10" location=":~:text=Meta%20robots%20%3A%20d%C3%A9finition%20et%20code%20HTML&amp;text=La%20meta%20meta%20robots%20est,la%20page%20(robots%20noindex)." ref="F11"/>
     <hyperlink r:id="rId11" ref="F12"/>
     <hyperlink r:id="rId12" ref="F13"/>
     <hyperlink r:id="rId13" ref="F14"/>
+    <hyperlink r:id="rId14" ref="F15"/>
+    <hyperlink r:id="rId15" ref="F16"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId14"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>